<commit_message>
total loss calc added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="332">
   <si>
     <t>ITB/10000002</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Fnol_PHDriverLicenseType</t>
   </si>
   <si>
-    <t>15/01/2019</t>
-  </si>
-  <si>
     <t>Fnol_TPDriverFirstName</t>
   </si>
   <si>
@@ -812,6 +809,219 @@
   </si>
   <si>
     <t>PostFnol_PropertyNewCompanyLocationDesc</t>
+  </si>
+  <si>
+    <t>ITB/10000000</t>
+  </si>
+  <si>
+    <t>Ainsley Lamb</t>
+  </si>
+  <si>
+    <t>NL68OXW</t>
+  </si>
+  <si>
+    <t>18/01/2019</t>
+  </si>
+  <si>
+    <t>10 Shillhope Drive, Blyth, NE24 4SN</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>other examples</t>
+  </si>
+  <si>
+    <t>Vehicle Damaged By Fire</t>
+  </si>
+  <si>
+    <t>Arson attack</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireWhenDate</t>
+  </si>
+  <si>
+    <t>18/01/2018</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireWhenTime</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireGarage</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireGarageDetails</t>
+  </si>
+  <si>
+    <t>It was in the garage last week for repairs</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireOtherVehicle</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireOtherVehicleDetails</t>
+  </si>
+  <si>
+    <t>The car next to mine was burnt</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireSuspected</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireSuspectNewPerson</t>
+  </si>
+  <si>
+    <t>todo..</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireWhySuspect</t>
+  </si>
+  <si>
+    <t>I saw them with a petrol bomb</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFireHowSuspectKnown</t>
+  </si>
+  <si>
+    <t>Unrelated</t>
+  </si>
+  <si>
+    <t>Theft</t>
+  </si>
+  <si>
+    <t>Theft Unrecovered</t>
+  </si>
+  <si>
+    <t>From locked garage</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftLastSeenDate</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftLastSeenTime</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftLossDate</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftLossTime</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftWindowsLocked</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftSecurityFitted</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftSecurityDetails</t>
+  </si>
+  <si>
+    <t>I have a crooklock</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftSecurityActive</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftKeysOnPurchase</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftKeysPossessed</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftKeyContactless</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftKeyLeftInVehicle</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftGarage</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftGarageDetails</t>
+  </si>
+  <si>
+    <t>It was in the garage last week for repairs AGAIN</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftSuspected</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftSuspectNewPerson</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftWhySuspect</t>
+  </si>
+  <si>
+    <t>I saw them with a crowbar</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftHowSuspectKnown</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftPoliceTreating</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftPoliceDetails</t>
+  </si>
+  <si>
+    <t>The police don’t believe it is stolen</t>
+  </si>
+  <si>
+    <t>I have just changedmy car in the last few weeks</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftVehicleChanged</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTheftVehicleChangedDetails</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFinanceOnVehicle</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFinanceMonthly</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFinanceMonthsRemaining</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleFinancePayOff</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleRoadWorthy</t>
+  </si>
+  <si>
+    <t>Exhaust Mods</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleModificationType</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleModified</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleNormallyKept</t>
+  </si>
+  <si>
+    <t>Residential Car Park</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleCurrentLocation</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleMileage</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCVehicleAge</t>
+  </si>
+  <si>
+    <t>3-6 years old</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleCallTotalLossCalc</t>
   </si>
 </sst>
 </file>
@@ -864,7 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -876,6 +1086,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1157,26 +1369,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B161"/>
+  <dimension ref="A1:I205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="E127" sqref="E126:E127"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1184,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1192,7 +1405,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1200,7 +1413,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1208,7 +1421,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1216,7 +1429,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="4"/>
     </row>
@@ -1225,7 +1438,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1241,7 +1454,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -1263,10 +1476,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1274,39 +1487,69 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1314,7 +1557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1322,7 +1565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1330,7 +1573,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1346,7 +1589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1354,7 +1597,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1362,7 +1605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1378,7 +1621,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1386,7 +1629,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1396,79 +1639,87 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
+      <c r="A35" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>92</v>
+      <c r="A36" s="8" t="s">
+        <v>322</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>93</v>
+      <c r="A37" s="8" t="s">
+        <v>324</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B38" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" t="b">
-        <v>1</v>
+      <c r="A39" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B39">
+        <v>17000</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" t="b">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" t="s">
-        <v>58</v>
+        <v>320</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>101</v>
+      <c r="A44" s="6" t="s">
+        <v>331</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -1476,474 +1727,493 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>329</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" t="s">
-        <v>129</v>
+        <v>316</v>
+      </c>
+      <c r="B46" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" t="s">
-        <v>104</v>
+        <v>317</v>
+      </c>
+      <c r="B47">
+        <v>125.66</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>161</v>
-      </c>
-      <c r="B48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="B48">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>162</v>
-      </c>
-      <c r="B49" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>164</v>
-      </c>
-      <c r="B50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="6" t="s">
-        <v>51</v>
+        <v>319</v>
+      </c>
+      <c r="B49">
+        <v>2476.44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>272</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>273</v>
       </c>
       <c r="B52" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>274</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>180</v>
-      </c>
-      <c r="B54" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+      <c r="B54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>277</v>
       </c>
       <c r="B55" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>205</v>
-      </c>
-      <c r="B57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>206</v>
+        <v>282</v>
       </c>
       <c r="B58" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>182</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>183</v>
-      </c>
-      <c r="B60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>284</v>
+      </c>
+      <c r="B59" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>184</v>
-      </c>
-      <c r="B61" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>290</v>
+      </c>
+      <c r="B61" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>185</v>
-      </c>
-      <c r="B62" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>186</v>
-      </c>
-      <c r="B63" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+      <c r="B63" s="9">
+        <v>0.33680555555555558</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>187</v>
-      </c>
-      <c r="B64" t="b">
+        <v>293</v>
+      </c>
+      <c r="B64" s="9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>188</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+      <c r="B65" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>189</v>
-      </c>
-      <c r="B66" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="6"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>297</v>
+      </c>
+      <c r="B67" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>298</v>
+      </c>
+      <c r="B68" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+      <c r="B69" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+      <c r="B70" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+      <c r="B71" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>302</v>
+      </c>
+      <c r="B72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>303</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="B74" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>315</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>82</v>
-      </c>
-      <c r="B76" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+      <c r="B76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>106</v>
-      </c>
-      <c r="B77" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>307</v>
       </c>
       <c r="B78" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>309</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>310</v>
+      </c>
+      <c r="B80" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>66</v>
-      </c>
-      <c r="B82" t="s">
-        <v>67</v>
+      <c r="A81" t="s">
+        <v>311</v>
+      </c>
+      <c r="B81" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>62</v>
-      </c>
-      <c r="B83" t="s">
-        <v>63</v>
+      <c r="A83" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>65</v>
-      </c>
-      <c r="B84" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="B84" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>208</v>
-      </c>
-      <c r="B85" t="b">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="B85" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>209</v>
+        <v>57</v>
       </c>
       <c r="B86" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="B87" t="s">
-        <v>207</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>69</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>68</v>
+        <v>100</v>
+      </c>
+      <c r="B88" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>96</v>
-      </c>
-      <c r="B89" t="b">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="B89" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>100</v>
-      </c>
-      <c r="B92" t="s">
-        <v>98</v>
+        <v>160</v>
+      </c>
+      <c r="B92" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>165</v>
-      </c>
-      <c r="B93" t="b">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="B93" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>166</v>
-      </c>
-      <c r="B94" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>167</v>
-      </c>
-      <c r="B95" t="b">
-        <v>0</v>
+        <v>163</v>
+      </c>
+      <c r="B94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B96" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B97" t="b">
-        <v>1</v>
+      <c r="A97" t="s">
+        <v>178</v>
+      </c>
+      <c r="B97" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="B98" t="s">
-        <v>67</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>151</v>
-      </c>
-      <c r="B100" t="s">
-        <v>158</v>
+        <v>203</v>
+      </c>
+      <c r="B100" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>200</v>
-      </c>
-      <c r="B101" t="b">
-        <v>1</v>
+        <v>204</v>
+      </c>
+      <c r="B101" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>202</v>
-      </c>
-      <c r="B103" t="s">
-        <v>203</v>
+        <v>181</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>152</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>159</v>
+        <v>182</v>
+      </c>
+      <c r="B104" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>153</v>
-      </c>
-      <c r="B105" t="b">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="B105" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="B106" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
         <v>97</v>
@@ -1951,409 +2221,740 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>156</v>
-      </c>
-      <c r="B108" t="s">
-        <v>98</v>
+        <v>186</v>
+      </c>
+      <c r="B108" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>168</v>
-      </c>
-      <c r="B109" t="b">
-        <v>0</v>
+        <v>187</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>169</v>
-      </c>
-      <c r="B110" t="s">
-        <v>163</v>
+        <v>188</v>
+      </c>
+      <c r="B110" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>170</v>
-      </c>
-      <c r="B111" t="b">
-        <v>0</v>
+      <c r="A111" s="6"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B112" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B113" t="b">
-        <v>1</v>
+      <c r="A113" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>110</v>
-      </c>
-      <c r="B115" t="s">
-        <v>116</v>
+        <v>72</v>
+      </c>
+      <c r="B115">
+        <v>2017</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>197</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B117" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>198</v>
+        <v>78</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>199</v>
+        <v>80</v>
       </c>
       <c r="B119" t="s">
-        <v>196</v>
+        <v>82</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>111</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>118</v>
+        <v>81</v>
+      </c>
+      <c r="B120" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>121</v>
-      </c>
-      <c r="B121">
-        <v>1237771234</v>
+        <v>105</v>
+      </c>
+      <c r="B121" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="B122" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>112</v>
-      </c>
-      <c r="B123" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>124</v>
-      </c>
-      <c r="B124" t="s">
-        <v>125</v>
+        <v>89</v>
+      </c>
+      <c r="B123" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
-        <v>113</v>
-      </c>
-      <c r="B125" t="s">
-        <v>119</v>
+      <c r="A125" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B125" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="B126" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>171</v>
-      </c>
-      <c r="B127" t="b">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="B127" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>64</v>
       </c>
       <c r="B128" t="s">
-        <v>163</v>
+        <v>63</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="B129" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>208</v>
+      </c>
+      <c r="B130" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B131" t="b">
-        <v>1</v>
+      <c r="A131" t="s">
+        <v>209</v>
+      </c>
+      <c r="B131" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>130</v>
-      </c>
-      <c r="B132" t="s">
-        <v>131</v>
+        <v>68</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>132</v>
-      </c>
-      <c r="B133" t="s">
-        <v>133</v>
+        <v>95</v>
+      </c>
+      <c r="B133" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>134</v>
-      </c>
-      <c r="B134">
-        <v>4000</v>
+        <v>125</v>
+      </c>
+      <c r="B134" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="B135" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="B136" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="B137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B138" t="s">
-        <v>67</v>
+        <v>194</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>141</v>
-      </c>
-      <c r="B139" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
-        <v>142</v>
-      </c>
-      <c r="B140" t="s">
-        <v>144</v>
+        <v>166</v>
+      </c>
+      <c r="B139" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
-        <v>147</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>148</v>
+      <c r="A141" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B141" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>146</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>149</v>
+      </c>
+      <c r="B143" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B144" t="b">
+      <c r="A144" t="s">
+        <v>150</v>
+      </c>
+      <c r="B144" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>199</v>
+      </c>
+      <c r="B145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>200</v>
+      </c>
+      <c r="B146" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>201</v>
+      </c>
+      <c r="B147" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>151</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>152</v>
+      </c>
+      <c r="B149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>153</v>
+      </c>
+      <c r="B150" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>155</v>
+      </c>
+      <c r="B152" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>167</v>
+      </c>
+      <c r="B153" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B145" t="b">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>168</v>
+      </c>
+      <c r="B154" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>169</v>
+      </c>
+      <c r="B155" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="6"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B147" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B149" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B154" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B155" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B156" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>226</v>
+      <c r="A157" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B157" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="8" t="s">
-        <v>228</v>
+      <c r="A158" t="s">
+        <v>107</v>
       </c>
       <c r="B158" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="8" t="s">
-        <v>230</v>
+      <c r="A159" t="s">
+        <v>109</v>
       </c>
       <c r="B159" t="s">
-        <v>231</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="8"/>
+      <c r="A160" t="s">
+        <v>108</v>
+      </c>
+      <c r="B160" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>196</v>
+      </c>
+      <c r="B161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>197</v>
+      </c>
+      <c r="B162" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>198</v>
+      </c>
+      <c r="B163" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>110</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>120</v>
+      </c>
+      <c r="B165">
+        <v>1237771234</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>121</v>
+      </c>
+      <c r="B166" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>111</v>
+      </c>
+      <c r="B167" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>123</v>
+      </c>
+      <c r="B168" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>112</v>
+      </c>
+      <c r="B169" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>113</v>
+      </c>
+      <c r="B170" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+      <c r="B171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>172</v>
+      </c>
+      <c r="B173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>129</v>
+      </c>
+      <c r="B176" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>131</v>
+      </c>
+      <c r="B177" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>133</v>
+      </c>
+      <c r="B178">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>134</v>
+      </c>
+      <c r="B179" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>136</v>
+      </c>
+      <c r="B180" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>138</v>
+      </c>
+      <c r="B181" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>139</v>
+      </c>
+      <c r="B182" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>140</v>
+      </c>
+      <c r="B183" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>141</v>
+      </c>
+      <c r="B184" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>146</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>144</v>
+      </c>
+      <c r="B186" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B188" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" s="6"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B193" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B198" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B199" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B200" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B202" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B203" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="8"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
         <v>6</v>
       </c>
-      <c r="B161" s="3" t="s">
-        <v>244</v>
+      <c r="B205" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B88" r:id="rId1"/>
-    <hyperlink ref="B120" r:id="rId2"/>
-    <hyperlink ref="B141" r:id="rId3"/>
-    <hyperlink ref="B104" r:id="rId4"/>
-    <hyperlink ref="B59" r:id="rId5"/>
+    <hyperlink ref="B132" r:id="rId1"/>
+    <hyperlink ref="B164" r:id="rId2"/>
+    <hyperlink ref="B185" r:id="rId3"/>
+    <hyperlink ref="B148" r:id="rId4"/>
+    <hyperlink ref="B103" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -2704,7 +3305,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2712,20 +3313,20 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6" s="2">
         <v>0.41666666666666669</v>
@@ -2733,39 +3334,39 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B11" s="3" t="b">
         <v>1</v>
@@ -2773,7 +3374,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12" s="3" t="b">
         <v>1</v>
@@ -2781,7 +3382,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13" s="3" t="b">
         <v>1</v>
@@ -2789,47 +3390,47 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B20">
         <v>4000</v>
@@ -2837,23 +3438,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -2861,47 +3462,47 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -2909,26 +3510,26 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>256</v>
+      </c>
+      <c r="B30" t="s">
         <v>257</v>
-      </c>
-      <c r="B30" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add story 210 tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="409">
   <si>
     <t>ITB/10000002</t>
   </si>
@@ -820,9 +820,6 @@
     <t>NL68OXW</t>
   </si>
   <si>
-    <t>18/01/2019</t>
-  </si>
-  <si>
     <t>10 Shillhope Drive, Blyth, NE24 4SN</t>
   </si>
   <si>
@@ -841,9 +838,6 @@
     <t>Fnol_PHVehicleFireWhenDate</t>
   </si>
   <si>
-    <t>18/01/2018</t>
-  </si>
-  <si>
     <t>Fnol_PHVehicleFireWhenTime</t>
   </si>
   <si>
@@ -1022,6 +1016,243 @@
   </si>
   <si>
     <t>Fnol_PHVehicleCallTotalLossCalc</t>
+  </si>
+  <si>
+    <t>The following drive the main screens which are used in FNOL</t>
+  </si>
+  <si>
+    <t>Almost all claims will need this</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_Step3_PHVehicleRequired is TRUE</t>
+  </si>
+  <si>
+    <t>Determines if the PH vehicle Total Loss cal subscreen is invoked</t>
+  </si>
+  <si>
+    <t>The following will only be used as part of PH vehicle if Fnol_PHVehicleCallTotalLossCalc is TRUE</t>
+  </si>
+  <si>
+    <t>The Fire subsection will only be shown if it’s a Fire incident type</t>
+  </si>
+  <si>
+    <t>The Theft subsection will only be shown if it’s a Theft incident type</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_PHDriverRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_PHPassengerRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_Step3_TPVehicleRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_TPDriverRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_TPPassengerRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_Step3_PedestrianRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_Step3_PropertyRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used  if Fnol_Step3_WitnessRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The following will only be used if Fnol_Step3_OfficialRequired is TRUE</t>
+  </si>
+  <si>
+    <t>The followign will only be used if Fnol_Step3_PoliceRequired is TRUE</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCAirbags</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCRollover</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCCosmetic</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCOver100k</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCLight</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCMedium</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCHeavy</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCVeryHeavy</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCBurnEngine</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCBurnInterior</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCDrivenWater</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCSubmerged</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCWaterInCompartment</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCWaterSeats</t>
+  </si>
+  <si>
+    <t>Fnol_PHVehicleTLCPointsTotal</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>21/01/2019</t>
+  </si>
+  <si>
+    <t>21/01/2018</t>
+  </si>
+  <si>
+    <t>Surveillance R us  - mr King 0777777788</t>
+  </si>
+  <si>
+    <t>Commercial Travelling</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncidentType</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_Cause</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_SubCause</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_FaulltRate</t>
+  </si>
+  <si>
+    <t>Fault</t>
+  </si>
+  <si>
+    <t>A Horse came round the corner</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_Circumstances</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_InsuredsLiability</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncUsingFor</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncPurpose</t>
+  </si>
+  <si>
+    <t>Had to get some files from work AGAIN</t>
+  </si>
+  <si>
+    <t>He WAS a friend of mine</t>
+  </si>
+  <si>
+    <t>61-70 MPH</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncKnowOtherDriver</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncNatureOfRel</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncSpeedImpact</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncWeather</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncRoadCond</t>
+  </si>
+  <si>
+    <t>Snow Covered</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncPhotos</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncCctv</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncCctvContact</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncPostcode</t>
+  </si>
+  <si>
+    <t>PostFnol_LossDetails_IncLocDesc</t>
+  </si>
+  <si>
+    <t>NE31UL</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianPrefix</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianFirstName</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianLastName</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianPostcodeSearch</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianPostcode</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianPostcodeAddress</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianEmail</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianMobile</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianNotes</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInjured</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInjDesc</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInj1BodyArea</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInj1Detailed</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInjHospAttend</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInjHospSearchName</t>
+  </si>
+  <si>
+    <t>PostFnol_PedestrianInjHospOvernight</t>
   </si>
 </sst>
 </file>
@@ -1369,30 +1600,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I205"/>
+  <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.1796875" customWidth="1"/>
     <col min="2" max="2" width="53.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1400,7 +1631,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1639,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1416,999 +1647,1077 @@
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>284</v>
+      </c>
+      <c r="D35" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>285</v>
+      </c>
+      <c r="D36" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
         <v>286</v>
       </c>
-      <c r="D19" t="s">
-        <v>266</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="D37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>287</v>
-      </c>
-      <c r="D20" t="s">
-        <v>268</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>288</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B52" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B53" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B54" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B55">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>318</v>
+      </c>
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>314</v>
+      </c>
+      <c r="B60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>315</v>
+      </c>
+      <c r="B61">
+        <v>125.66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>316</v>
+      </c>
+      <c r="B62">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>317</v>
+      </c>
+      <c r="B63">
+        <v>2476.44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="B35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B36" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B37" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B38" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="B39">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>320</v>
-      </c>
-      <c r="B42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="B44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>329</v>
-      </c>
-      <c r="B45" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>316</v>
-      </c>
-      <c r="B46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>317</v>
-      </c>
-      <c r="B47">
-        <v>125.66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>318</v>
-      </c>
-      <c r="B48">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>319</v>
-      </c>
-      <c r="B49">
-        <v>2476.44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>272</v>
-      </c>
-      <c r="B51" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>273</v>
-      </c>
-      <c r="B52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>274</v>
-      </c>
-      <c r="B53" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>276</v>
-      </c>
-      <c r="B54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>277</v>
-      </c>
-      <c r="B55" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>279</v>
-      </c>
-      <c r="B56" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>280</v>
-      </c>
-      <c r="B57" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>282</v>
-      </c>
-      <c r="B58" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>284</v>
-      </c>
-      <c r="B59" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>290</v>
-      </c>
-      <c r="B61" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>291</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>292</v>
-      </c>
-      <c r="B63" s="9">
-        <v>0.33680555555555558</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>293</v>
-      </c>
-      <c r="B64" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>294</v>
-      </c>
-      <c r="B65" s="9" t="b">
-        <v>1</v>
+      <c r="B65" s="3" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>295</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>296</v>
+        <v>270</v>
+      </c>
+      <c r="B66" s="9">
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>297</v>
-      </c>
-      <c r="B67" s="9" t="b">
+        <v>271</v>
+      </c>
+      <c r="B67" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>298</v>
-      </c>
-      <c r="B68" s="10">
-        <v>3</v>
+        <v>272</v>
+      </c>
+      <c r="B68" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>299</v>
-      </c>
-      <c r="B69" s="10">
-        <v>2</v>
+        <v>274</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>300</v>
-      </c>
-      <c r="B70" s="10" t="b">
-        <v>1</v>
+        <v>275</v>
+      </c>
+      <c r="B70" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>301</v>
-      </c>
-      <c r="B71" s="10" t="b">
-        <v>0</v>
+        <v>277</v>
+      </c>
+      <c r="B71" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="B72" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="B73" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>314</v>
-      </c>
-      <c r="B74" s="10" t="b">
-        <v>1</v>
+        <v>282</v>
+      </c>
+      <c r="B74" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>315</v>
-      </c>
-      <c r="B75" t="s">
-        <v>313</v>
+      <c r="A75" s="6" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>305</v>
-      </c>
-      <c r="B76" t="b">
-        <v>1</v>
+      <c r="A76" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>306</v>
-      </c>
-      <c r="B77" t="b">
-        <v>0</v>
-      </c>
-      <c r="D77" t="s">
-        <v>281</v>
+        <v>288</v>
+      </c>
+      <c r="B77" s="9">
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>307</v>
-      </c>
-      <c r="B78" t="s">
-        <v>308</v>
+        <v>289</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>309</v>
-      </c>
-      <c r="B79" t="s">
-        <v>285</v>
+        <v>290</v>
+      </c>
+      <c r="B79" s="9">
+        <v>0.33680555555555558</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>291</v>
+      </c>
+      <c r="B80" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>292</v>
+      </c>
+      <c r="B81" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>293</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>295</v>
+      </c>
+      <c r="B83" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>296</v>
+      </c>
+      <c r="B84" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>297</v>
+      </c>
+      <c r="B85" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>298</v>
+      </c>
+      <c r="B86" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>299</v>
+      </c>
+      <c r="B87" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>300</v>
+      </c>
+      <c r="B88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>301</v>
+      </c>
+      <c r="B89" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>312</v>
+      </c>
+      <c r="B90" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>313</v>
+      </c>
+      <c r="B91" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>303</v>
+      </c>
+      <c r="B92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>304</v>
+      </c>
+      <c r="B93" t="b">
+        <v>0</v>
+      </c>
+      <c r="D93" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>305</v>
+      </c>
+      <c r="B94" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>307</v>
+      </c>
+      <c r="B95" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>308</v>
+      </c>
+      <c r="B96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>309</v>
+      </c>
+      <c r="B97" t="s">
         <v>310</v>
       </c>
-      <c r="B80" t="b">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>327</v>
+      </c>
+      <c r="B99" t="s">
+        <v>328</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>350</v>
+      </c>
+      <c r="B100" t="b">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>15</v>
+      </c>
+      <c r="D100" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>347</v>
+      </c>
+      <c r="B101" t="s">
+        <v>93</v>
+      </c>
+      <c r="C101">
+        <v>15</v>
+      </c>
+      <c r="D101" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>348</v>
+      </c>
+      <c r="B102" t="b">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>25</v>
+      </c>
+      <c r="D102" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>349</v>
+      </c>
+      <c r="B103" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>311</v>
-      </c>
-      <c r="B81" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B83" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>351</v>
+      </c>
+      <c r="B104" t="b">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>352</v>
+      </c>
+      <c r="B105" t="b">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>353</v>
+      </c>
+      <c r="B106" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>354</v>
+      </c>
+      <c r="B107" t="b">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>20</v>
+      </c>
+      <c r="D107" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>355</v>
+      </c>
+      <c r="B108" t="b">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>20</v>
+      </c>
+      <c r="D108" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>356</v>
+      </c>
+      <c r="B109" t="b">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>25</v>
+      </c>
+      <c r="D109" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>357</v>
+      </c>
+      <c r="B110" t="b">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>20</v>
+      </c>
+      <c r="D110" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>358</v>
+      </c>
+      <c r="B111" t="b">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>25</v>
+      </c>
+      <c r="D111" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>359</v>
+      </c>
+      <c r="B112" t="b">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>15</v>
+      </c>
+      <c r="D112" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>360</v>
+      </c>
+      <c r="B113" t="b">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <v>25</v>
+      </c>
+      <c r="D113" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>361</v>
+      </c>
+      <c r="B114">
+        <v>210</v>
+      </c>
+      <c r="C114">
+        <f>SUM(C99:C113)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>54</v>
       </c>
-      <c r="B84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="B117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>55</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B118" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>57</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B119" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>60</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B120" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>100</v>
       </c>
-      <c r="B88" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+      <c r="B121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>101</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B122" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>127</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B123" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>104</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B124" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>160</v>
       </c>
-      <c r="B92" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="B125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>161</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B126" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>163</v>
       </c>
-      <c r="B94" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B96" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>178</v>
-      </c>
-      <c r="B97" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>179</v>
-      </c>
-      <c r="B98" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>180</v>
-      </c>
-      <c r="B99" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>203</v>
-      </c>
-      <c r="B100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>204</v>
-      </c>
-      <c r="B101" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>205</v>
-      </c>
-      <c r="B102" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>181</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>182</v>
-      </c>
-      <c r="B104" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>183</v>
-      </c>
-      <c r="B105" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>184</v>
-      </c>
-      <c r="B106" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>185</v>
-      </c>
-      <c r="B107" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
-        <v>186</v>
-      </c>
-      <c r="B108" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>187</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
-        <v>188</v>
-      </c>
-      <c r="B110" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="6"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B112" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>69</v>
-      </c>
-      <c r="B113" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>71</v>
-      </c>
-      <c r="B114" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>72</v>
-      </c>
-      <c r="B115">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
-        <v>73</v>
-      </c>
-      <c r="B116" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>74</v>
-      </c>
-      <c r="B117" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>78</v>
-      </c>
-      <c r="B118" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
-        <v>80</v>
-      </c>
-      <c r="B119" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
-        <v>81</v>
-      </c>
-      <c r="B120" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
-        <v>105</v>
-      </c>
-      <c r="B121" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
-        <v>88</v>
-      </c>
-      <c r="B122" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
-        <v>89</v>
-      </c>
-      <c r="B123" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B125" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
-        <v>65</v>
-      </c>
-      <c r="B126" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
-        <v>61</v>
-      </c>
-      <c r="B127" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>64</v>
-      </c>
-      <c r="B128" t="s">
-        <v>63</v>
+      <c r="B127" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
-        <v>207</v>
-      </c>
-      <c r="B129" t="b">
-        <v>1</v>
+      <c r="A129" s="6" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="B131" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>68</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>67</v>
+        <v>180</v>
+      </c>
+      <c r="B132" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="B133" t="b">
         <v>1</v>
@@ -2416,545 +2725,775 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>125</v>
+        <v>204</v>
       </c>
       <c r="B134" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="B135" t="s">
-        <v>96</v>
+        <v>202</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>99</v>
-      </c>
-      <c r="B136" t="s">
-        <v>97</v>
+        <v>181</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="B137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="B138" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>166</v>
-      </c>
-      <c r="B139" t="b">
+        <v>184</v>
+      </c>
+      <c r="B139" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>185</v>
+      </c>
+      <c r="B140" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>186</v>
+      </c>
+      <c r="B141" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B141" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>148</v>
-      </c>
-      <c r="B142" t="s">
-        <v>66</v>
+        <v>187</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>149</v>
-      </c>
-      <c r="B143" t="s">
-        <v>156</v>
+        <v>188</v>
+      </c>
+      <c r="B143" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>150</v>
-      </c>
-      <c r="B144" t="s">
-        <v>157</v>
-      </c>
+      <c r="A144" s="6"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
-        <v>199</v>
-      </c>
-      <c r="B145" t="b">
-        <v>1</v>
+      <c r="A145" s="6" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>200</v>
+        <v>69</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>201</v>
+        <v>71</v>
       </c>
       <c r="B147" t="s">
-        <v>202</v>
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>151</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>158</v>
+        <v>72</v>
+      </c>
+      <c r="B148">
+        <v>2017</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>152</v>
-      </c>
-      <c r="B149" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="B149" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="B150" t="s">
-        <v>159</v>
+        <v>77</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>154</v>
+        <v>78</v>
       </c>
       <c r="B151" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="B152" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>167</v>
-      </c>
-      <c r="B153" t="b">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="B153" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>105</v>
       </c>
       <c r="B154" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>169</v>
-      </c>
-      <c r="B155" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B157" t="b">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="B155" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>89</v>
+      </c>
+      <c r="B156" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
-        <v>107</v>
-      </c>
-      <c r="B158" t="s">
-        <v>114</v>
+      <c r="A158" s="6" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="B160" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>196</v>
-      </c>
-      <c r="B161" t="b">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="B161" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>197</v>
-      </c>
-      <c r="B162" t="s">
-        <v>25</v>
+        <v>207</v>
+      </c>
+      <c r="B162" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B163" t="s">
-        <v>195</v>
+        <v>25</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>110</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>117</v>
+        <v>209</v>
+      </c>
+      <c r="B164" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>120</v>
-      </c>
-      <c r="B165">
-        <v>1237771234</v>
+        <v>68</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>121</v>
-      </c>
-      <c r="B166" t="s">
-        <v>122</v>
+        <v>95</v>
+      </c>
+      <c r="B166" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>111</v>
-      </c>
-      <c r="B167" t="b">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="B167" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B168" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B169" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>113</v>
-      </c>
-      <c r="B170" t="s">
-        <v>119</v>
+        <v>164</v>
+      </c>
+      <c r="B170" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>170</v>
-      </c>
-      <c r="B171" t="b">
-        <v>0</v>
+        <v>165</v>
+      </c>
+      <c r="B171" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>171</v>
-      </c>
-      <c r="B172" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
-        <v>172</v>
-      </c>
-      <c r="B173" t="b">
+        <v>166</v>
+      </c>
+      <c r="B172" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B175" t="b">
-        <v>1</v>
+      <c r="A175" t="s">
+        <v>148</v>
+      </c>
+      <c r="B175" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="B176" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B177" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>133</v>
-      </c>
-      <c r="B178">
-        <v>4000</v>
+        <v>199</v>
+      </c>
+      <c r="B178" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
       <c r="B179" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="B180" t="s">
-        <v>137</v>
+        <v>202</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>138</v>
-      </c>
-      <c r="B181" t="b">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>139</v>
-      </c>
-      <c r="B182" t="s">
-        <v>66</v>
+        <v>152</v>
+      </c>
+      <c r="B182" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B183" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="B184" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>146</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>147</v>
+        <v>155</v>
+      </c>
+      <c r="B185" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>144</v>
-      </c>
-      <c r="B186" t="s">
-        <v>145</v>
+        <v>167</v>
+      </c>
+      <c r="B186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>168</v>
+      </c>
+      <c r="B187" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" s="6" t="s">
-        <v>47</v>
+      <c r="A188" t="s">
+        <v>169</v>
       </c>
       <c r="B188" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B189" t="b">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>107</v>
+      </c>
+      <c r="B191" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>109</v>
+      </c>
+      <c r="B192" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>108</v>
+      </c>
+      <c r="B193" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>196</v>
+      </c>
+      <c r="B194" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>197</v>
+      </c>
+      <c r="B195" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>198</v>
+      </c>
+      <c r="B196" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>110</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>120</v>
+      </c>
+      <c r="B198">
+        <v>1237771234</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>121</v>
+      </c>
+      <c r="B199" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>111</v>
+      </c>
+      <c r="B200" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>123</v>
+      </c>
+      <c r="B201" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>112</v>
+      </c>
+      <c r="B202" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>113</v>
+      </c>
+      <c r="B203" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>170</v>
+      </c>
+      <c r="B204" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="6"/>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B191" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B193" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A194" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A195" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A198" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B198" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B199" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A200" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B200" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A202" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B202" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="B203" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" s="8"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
+        <v>171</v>
+      </c>
+      <c r="B205" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>172</v>
+      </c>
+      <c r="B206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>129</v>
+      </c>
+      <c r="B209" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>131</v>
+      </c>
+      <c r="B210" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>133</v>
+      </c>
+      <c r="B211">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>134</v>
+      </c>
+      <c r="B212" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>136</v>
+      </c>
+      <c r="B213" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>138</v>
+      </c>
+      <c r="B214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>139</v>
+      </c>
+      <c r="B215" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>140</v>
+      </c>
+      <c r="B216" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>141</v>
+      </c>
+      <c r="B217" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>146</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>144</v>
+      </c>
+      <c r="B219" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" s="6"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="6"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B227" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B232" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B233" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B234" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B236" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B237" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="8"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
         <v>6</v>
       </c>
-      <c r="B205" s="3" t="s">
+      <c r="B239" s="3" t="s">
         <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B132" r:id="rId1"/>
-    <hyperlink ref="B164" r:id="rId2"/>
-    <hyperlink ref="B185" r:id="rId3"/>
-    <hyperlink ref="B148" r:id="rId4"/>
-    <hyperlink ref="B103" r:id="rId5"/>
+    <hyperlink ref="B165" r:id="rId1"/>
+    <hyperlink ref="B197" r:id="rId2"/>
+    <hyperlink ref="B218" r:id="rId3"/>
+    <hyperlink ref="B181" r:id="rId4"/>
+    <hyperlink ref="B136" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -3291,24 +3830,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3316,228 +3855,531 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="B11" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="B12" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="B13" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>241</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>375</v>
+      </c>
+      <c r="B12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>381</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>242</v>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>382</v>
       </c>
       <c r="B16" t="s">
-        <v>230</v>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>383</v>
+      </c>
+      <c r="B17" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>384</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>387</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>246</v>
-      </c>
-      <c r="B20">
-        <v>4000</v>
+        <v>388</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>389</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B22" t="s">
-        <v>137</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>249</v>
-      </c>
-      <c r="B23" t="b">
-        <v>1</v>
+        <v>390</v>
+      </c>
+      <c r="B23" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>391</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B32" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B34" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>244</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>245</v>
+      </c>
+      <c r="B40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>246</v>
+      </c>
+      <c r="B41">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>247</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>250</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>251</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B46" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>252</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B47" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>253</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>254</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B49" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>255</v>
       </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>256</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B51" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>258</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>260</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B53" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>393</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>394</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>395</v>
+      </c>
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>396</v>
+      </c>
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>397</v>
+      </c>
+      <c r="B59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>398</v>
+      </c>
+      <c r="B60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>399</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>400</v>
+      </c>
+      <c r="B62">
+        <v>1237771234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>401</v>
+      </c>
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>402</v>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>403</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>404</v>
+      </c>
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>405</v>
+      </c>
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>406</v>
+      </c>
+      <c r="B68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>407</v>
+      </c>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>408</v>
+      </c>
+      <c r="B70" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B27" r:id="rId1"/>
-    <hyperlink ref="B31" r:id="rId2"/>
+    <hyperlink ref="B48" r:id="rId1"/>
+    <hyperlink ref="B52" r:id="rId2"/>
+    <hyperlink ref="B61" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test for stort 216 added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="412">
   <si>
     <t>ITB/10000002</t>
   </si>
@@ -757,9 +757,6 @@
     <t>PostFnol_PoliceForceSearchName</t>
   </si>
   <si>
-    <t>000-00-000033</t>
-  </si>
-  <si>
     <t>PostFnol_PropertyDesc</t>
   </si>
   <si>
@@ -1253,6 +1250,18 @@
   </si>
   <si>
     <t>PostFnol_PedestrianInjHospOvernight</t>
+  </si>
+  <si>
+    <t>000-00-000032</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_AlertNotified</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_AlertId</t>
+  </si>
+  <si>
+    <t>TBX59595959</t>
   </si>
 </sst>
 </file>
@@ -1600,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I239"/>
+  <dimension ref="A1:I241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1628,7 +1637,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1636,7 +1645,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1644,7 +1653,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1652,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1660,7 +1669,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" s="4"/>
     </row>
@@ -1672,18 +1681,18 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B10" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1786,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1822,95 +1831,95 @@
         <v>19</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>409</v>
+      </c>
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="A32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B32" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>284</v>
-      </c>
-      <c r="D35" t="s">
-        <v>265</v>
-      </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" t="s">
-        <v>284</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>285</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>267</v>
-      </c>
-      <c r="E36" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D37" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I37" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>284</v>
+      </c>
+      <c r="D38" t="s">
+        <v>266</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>285</v>
+      </c>
+      <c r="D39" t="s">
+        <v>267</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -1923,148 +1932,148 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="B43" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="B51" t="b">
-        <v>1</v>
-      </c>
-    </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="B52" t="s">
-        <v>319</v>
+      <c r="A52" s="6" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B53" t="s">
-        <v>323</v>
+        <v>320</v>
+      </c>
+      <c r="B53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B54" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B55">
+        <v>321</v>
+      </c>
+      <c r="B55" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B56" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B57">
         <v>17000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>318</v>
-      </c>
-      <c r="B58" t="b">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B60" t="b">
         <v>1</v>
@@ -2072,68 +2081,68 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>315</v>
-      </c>
-      <c r="B61">
-        <v>125.66</v>
+        <v>92</v>
+      </c>
+      <c r="B61" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>316</v>
-      </c>
-      <c r="B62">
-        <v>13</v>
+        <v>313</v>
+      </c>
+      <c r="B62" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B63">
+        <v>125.66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>315</v>
+      </c>
+      <c r="B64">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>316</v>
+      </c>
+      <c r="B65">
         <v>2476.44</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>270</v>
-      </c>
-      <c r="B66" s="9">
-        <v>0.33333333333333331</v>
+      <c r="A66" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>271</v>
-      </c>
-      <c r="B67" t="b">
-        <v>1</v>
+      <c r="A67" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>272</v>
-      </c>
-      <c r="B68" t="s">
-        <v>273</v>
+        <v>269</v>
+      </c>
+      <c r="B68" s="9">
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -2141,15 +2150,15 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B70" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B71" t="b">
         <v>1</v>
@@ -2157,95 +2166,95 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>278</v>
-      </c>
-      <c r="B72" t="b">
-        <v>0</v>
-      </c>
-      <c r="D72" t="s">
-        <v>279</v>
+        <v>274</v>
+      </c>
+      <c r="B72" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>280</v>
-      </c>
-      <c r="B73" t="s">
-        <v>281</v>
+        <v>276</v>
+      </c>
+      <c r="B73" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>277</v>
+      </c>
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>279</v>
+      </c>
+      <c r="B75" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>281</v>
+      </c>
+      <c r="B76" t="s">
         <v>282</v>
       </c>
-      <c r="B74" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>364</v>
-      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B77" s="9">
-        <v>0.33333333333333331</v>
+      <c r="A77" s="6" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>289</v>
+      <c r="A78" s="8" t="s">
+        <v>286</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B79" s="9">
-        <v>0.33680555555555558</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>291</v>
-      </c>
-      <c r="B80" s="9" t="b">
-        <v>0</v>
+        <v>288</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>292</v>
-      </c>
-      <c r="B81" s="9" t="b">
-        <v>1</v>
+        <v>289</v>
+      </c>
+      <c r="B81" s="9">
+        <v>0.33680555555555558</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>293</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
+      </c>
+      <c r="B82" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B83" s="9" t="b">
         <v>1</v>
@@ -2253,211 +2262,199 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>296</v>
-      </c>
-      <c r="B84" s="10">
-        <v>3</v>
+        <v>292</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>297</v>
-      </c>
-      <c r="B85" s="10">
-        <v>2</v>
+        <v>294</v>
+      </c>
+      <c r="B85" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>298</v>
-      </c>
-      <c r="B86" s="10" t="b">
-        <v>1</v>
+        <v>295</v>
+      </c>
+      <c r="B86" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>299</v>
-      </c>
-      <c r="B87" s="10" t="b">
-        <v>0</v>
+        <v>296</v>
+      </c>
+      <c r="B87" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>300</v>
-      </c>
-      <c r="B88" t="b">
+        <v>297</v>
+      </c>
+      <c r="B88" s="10" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>301</v>
-      </c>
-      <c r="B89" t="s">
-        <v>302</v>
+        <v>298</v>
+      </c>
+      <c r="B89" s="10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>312</v>
-      </c>
-      <c r="B90" s="10" t="b">
+        <v>299</v>
+      </c>
+      <c r="B90" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B91" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>303</v>
-      </c>
-      <c r="B92" t="b">
+        <v>311</v>
+      </c>
+      <c r="B92" s="10" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>304</v>
-      </c>
-      <c r="B93" t="b">
-        <v>0</v>
-      </c>
-      <c r="D93" t="s">
-        <v>279</v>
+        <v>312</v>
+      </c>
+      <c r="B93" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>305</v>
-      </c>
-      <c r="B94" t="s">
-        <v>306</v>
+        <v>302</v>
+      </c>
+      <c r="B94" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>307</v>
-      </c>
-      <c r="B95" t="s">
-        <v>283</v>
+        <v>303</v>
+      </c>
+      <c r="B95" t="b">
+        <v>0</v>
+      </c>
+      <c r="D95" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>308</v>
-      </c>
-      <c r="B96" t="b">
-        <v>0</v>
+        <v>304</v>
+      </c>
+      <c r="B96" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B97" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" s="6" t="s">
-        <v>334</v>
+      <c r="A98" t="s">
+        <v>307</v>
+      </c>
+      <c r="B98" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="B99" t="s">
-        <v>328</v>
-      </c>
-      <c r="C99">
-        <v>5</v>
-      </c>
-      <c r="D99" t="s">
-        <v>362</v>
+        <v>309</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>350</v>
-      </c>
-      <c r="B100" t="b">
-        <v>1</v>
-      </c>
-      <c r="C100">
-        <v>15</v>
-      </c>
-      <c r="D100" t="s">
-        <v>362</v>
+      <c r="A100" s="6" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="B101" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="C101">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B102" t="b">
         <v>1</v>
       </c>
       <c r="C102">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>349</v>
-      </c>
-      <c r="B103" t="b">
-        <v>0</v>
+        <v>346</v>
+      </c>
+      <c r="B103" t="s">
+        <v>93</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D103" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D104" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B105" t="b">
         <v>0</v>
@@ -2466,12 +2463,12 @@
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B106" t="b">
         <v>0</v>
@@ -2480,54 +2477,54 @@
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B109" t="b">
         <v>1</v>
       </c>
       <c r="C109">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B110" t="b">
         <v>1</v>
@@ -2536,12 +2533,12 @@
         <v>20</v>
       </c>
       <c r="D110" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B111" t="b">
         <v>1</v>
@@ -2550,26 +2547,26 @@
         <v>25</v>
       </c>
       <c r="D111" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B112" t="b">
         <v>1</v>
       </c>
       <c r="C112">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D112" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B113" t="b">
         <v>1</v>
@@ -2578,798 +2575,818 @@
         <v>25</v>
       </c>
       <c r="D113" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>358</v>
+      </c>
+      <c r="B114" t="b">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>15</v>
+      </c>
+      <c r="D114" t="s">
         <v>361</v>
       </c>
-      <c r="B114">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>359</v>
+      </c>
+      <c r="B115" t="b">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>25</v>
+      </c>
+      <c r="D115" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>360</v>
+      </c>
+      <c r="B116">
         <v>210</v>
       </c>
-      <c r="C114">
-        <f>SUM(C99:C113)</f>
+      <c r="C116">
+        <f>SUM(C101:C115)</f>
         <v>210</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A116" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>54</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
-      </c>
-    </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>55</v>
-      </c>
-      <c r="B118" t="s">
-        <v>56</v>
+      <c r="A118" s="6" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>57</v>
-      </c>
-      <c r="B119" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="B119" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B120" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>100</v>
-      </c>
-      <c r="B121" t="b">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="B121" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="B122" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>127</v>
-      </c>
-      <c r="B123" t="s">
-        <v>128</v>
+        <v>100</v>
+      </c>
+      <c r="B123" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B124" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>160</v>
-      </c>
-      <c r="B125" t="b">
-        <v>1</v>
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="B126" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>160</v>
+      </c>
+      <c r="B127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>161</v>
+      </c>
+      <c r="B128" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>163</v>
       </c>
-      <c r="B127" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="6" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>178</v>
-      </c>
-      <c r="B130" t="s">
-        <v>66</v>
+      <c r="B129" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
-        <v>179</v>
-      </c>
-      <c r="B131" t="s">
-        <v>189</v>
+      <c r="A131" s="6" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B132" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>203</v>
-      </c>
-      <c r="B133" t="b">
-        <v>1</v>
+        <v>179</v>
+      </c>
+      <c r="B133" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>190</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>205</v>
-      </c>
-      <c r="B135" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="B135" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>181</v>
-      </c>
-      <c r="B136" s="5" t="s">
-        <v>191</v>
+        <v>204</v>
+      </c>
+      <c r="B136" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>182</v>
-      </c>
-      <c r="B137" t="b">
-        <v>1</v>
+        <v>205</v>
+      </c>
+      <c r="B137" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>183</v>
-      </c>
-      <c r="B138" t="s">
-        <v>192</v>
+        <v>181</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>184</v>
-      </c>
-      <c r="B139" t="s">
-        <v>96</v>
+        <v>182</v>
+      </c>
+      <c r="B139" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B140" t="s">
-        <v>97</v>
+        <v>192</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>186</v>
-      </c>
-      <c r="B141" t="b">
-        <v>0</v>
+        <v>184</v>
+      </c>
+      <c r="B141" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>187</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>193</v>
+        <v>185</v>
+      </c>
+      <c r="B142" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
+        <v>186</v>
+      </c>
+      <c r="B143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>187</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>188</v>
       </c>
-      <c r="B143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="6"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="6" t="s">
-        <v>339</v>
+      <c r="B145" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
-        <v>69</v>
-      </c>
-      <c r="B146" t="s">
-        <v>70</v>
-      </c>
+      <c r="A146" s="6"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
-        <v>71</v>
-      </c>
-      <c r="B147" t="s">
-        <v>75</v>
+      <c r="A147" s="6" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>72</v>
-      </c>
-      <c r="B148">
-        <v>2017</v>
+        <v>69</v>
+      </c>
+      <c r="B148" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B149" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>74</v>
-      </c>
-      <c r="B150" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="B150">
+        <v>2017</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B151" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B152" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B153" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="B154" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B155" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
+        <v>105</v>
+      </c>
+      <c r="B156" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>88</v>
+      </c>
+      <c r="B157" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>89</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B158" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="6" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
-        <v>65</v>
-      </c>
-      <c r="B159" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
-        <v>61</v>
-      </c>
-      <c r="B160" t="s">
-        <v>62</v>
+      <c r="A160" s="6" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B161" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>207</v>
-      </c>
-      <c r="B162" t="b">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="B162" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>208</v>
+        <v>64</v>
       </c>
       <c r="B163" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>209</v>
-      </c>
-      <c r="B164" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="B164" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>68</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>67</v>
+        <v>208</v>
+      </c>
+      <c r="B165" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>95</v>
-      </c>
-      <c r="B166" t="b">
-        <v>1</v>
+        <v>209</v>
+      </c>
+      <c r="B166" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>125</v>
-      </c>
-      <c r="B167" t="s">
-        <v>126</v>
+        <v>68</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>98</v>
-      </c>
-      <c r="B168" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="B168" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B169" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>164</v>
-      </c>
-      <c r="B170" t="b">
-        <v>0</v>
+        <v>98</v>
+      </c>
+      <c r="B170" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="B171" t="s">
-        <v>194</v>
+        <v>97</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B172" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>165</v>
+      </c>
+      <c r="B173" t="s">
+        <v>194</v>
+      </c>
+    </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="6" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
-        <v>148</v>
-      </c>
-      <c r="B175" t="s">
-        <v>66</v>
+      <c r="A174" t="s">
+        <v>166</v>
+      </c>
+      <c r="B174" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
-        <v>149</v>
-      </c>
-      <c r="B176" t="s">
-        <v>156</v>
+      <c r="A176" s="6" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B177" t="s">
-        <v>157</v>
+        <v>66</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>199</v>
-      </c>
-      <c r="B178" t="b">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="B178" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B179" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>201</v>
-      </c>
-      <c r="B180" t="s">
-        <v>202</v>
+        <v>199</v>
+      </c>
+      <c r="B180" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>151</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>158</v>
+        <v>200</v>
+      </c>
+      <c r="B181" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>152</v>
-      </c>
-      <c r="B182" t="b">
-        <v>1</v>
+        <v>201</v>
+      </c>
+      <c r="B182" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>153</v>
-      </c>
-      <c r="B183" t="s">
-        <v>159</v>
+        <v>151</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>154</v>
-      </c>
-      <c r="B184" t="s">
-        <v>96</v>
+        <v>152</v>
+      </c>
+      <c r="B184" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B185" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>167</v>
-      </c>
-      <c r="B186" t="b">
-        <v>0</v>
+        <v>154</v>
+      </c>
+      <c r="B186" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B187" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B188" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>168</v>
+      </c>
+      <c r="B189" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>107</v>
-      </c>
-      <c r="B191" t="s">
-        <v>114</v>
+      <c r="A190" t="s">
+        <v>169</v>
+      </c>
+      <c r="B190" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>109</v>
-      </c>
-      <c r="B192" t="s">
-        <v>115</v>
+      <c r="A192" s="6" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B193" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>196</v>
-      </c>
-      <c r="B194" t="b">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="B194" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>197</v>
+        <v>108</v>
       </c>
       <c r="B195" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>198</v>
-      </c>
-      <c r="B196" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="B196" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>110</v>
-      </c>
-      <c r="B197" s="5" t="s">
-        <v>117</v>
+        <v>197</v>
+      </c>
+      <c r="B197" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>120</v>
-      </c>
-      <c r="B198">
-        <v>1237771234</v>
+        <v>198</v>
+      </c>
+      <c r="B198" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>121</v>
-      </c>
-      <c r="B199" t="s">
-        <v>122</v>
+        <v>110</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>111</v>
-      </c>
-      <c r="B200" t="b">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B200">
+        <v>1237771234</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B201" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>112</v>
-      </c>
-      <c r="B202" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="B202" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B203" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>170</v>
-      </c>
-      <c r="B204" t="b">
-        <v>0</v>
+        <v>112</v>
+      </c>
+      <c r="B204" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="B205" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B206" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>171</v>
+      </c>
+      <c r="B207" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" t="s">
-        <v>129</v>
-      </c>
-      <c r="B209" t="s">
-        <v>130</v>
+      <c r="A208" t="s">
+        <v>172</v>
+      </c>
+      <c r="B208" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" t="s">
-        <v>131</v>
-      </c>
-      <c r="B210" t="s">
-        <v>132</v>
+      <c r="A210" s="6" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>133</v>
-      </c>
-      <c r="B211">
-        <v>4000</v>
+        <v>129</v>
+      </c>
+      <c r="B211" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B212" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>136</v>
-      </c>
-      <c r="B213" t="s">
-        <v>137</v>
+        <v>133</v>
+      </c>
+      <c r="B213">
+        <v>4000</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>138</v>
-      </c>
-      <c r="B214" t="b">
-        <v>1</v>
+        <v>134</v>
+      </c>
+      <c r="B214" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B215" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>140</v>
-      </c>
-      <c r="B216" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+      <c r="B216" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B217" t="s">
-        <v>143</v>
+        <v>66</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>146</v>
-      </c>
-      <c r="B218" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
+      </c>
+      <c r="B218" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
+        <v>141</v>
+      </c>
+      <c r="B219" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>146</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
         <v>144</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B221" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" s="6"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
@@ -3377,76 +3394,68 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A226" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="B226" s="3" t="s">
-        <v>212</v>
-      </c>
+      <c r="A226" s="6"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A227" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B227" s="2">
-        <v>0.41666666666666669</v>
+      <c r="A227" s="6" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B229" s="3" t="s">
-        <v>220</v>
+        <v>213</v>
+      </c>
+      <c r="B229" s="2">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B232" s="3" t="b">
-        <v>1</v>
+        <v>216</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B233" s="3" t="b">
-        <v>1</v>
+        <v>217</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" s="8" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B234" s="3" t="b">
         <v>1</v>
@@ -3454,46 +3463,62 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B235" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="B235" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B236" t="s">
-        <v>228</v>
+        <v>224</v>
+      </c>
+      <c r="B236" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B238" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B239" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A238" s="8"/>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" s="8"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
         <v>6</v>
       </c>
-      <c r="B239" s="3" t="s">
-        <v>243</v>
+      <c r="B241" s="3" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B165" r:id="rId1"/>
-    <hyperlink ref="B197" r:id="rId2"/>
-    <hyperlink ref="B218" r:id="rId3"/>
-    <hyperlink ref="B181" r:id="rId4"/>
-    <hyperlink ref="B136" r:id="rId5"/>
+    <hyperlink ref="B167" r:id="rId1"/>
+    <hyperlink ref="B199" r:id="rId2"/>
+    <hyperlink ref="B220" r:id="rId3"/>
+    <hyperlink ref="B183" r:id="rId4"/>
+    <hyperlink ref="B138" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -3832,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3852,7 +3877,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>243</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3860,74 +3885,74 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>369</v>
+      </c>
+      <c r="B9" t="s">
         <v>370</v>
-      </c>
-      <c r="B9" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B10">
         <v>75</v>
@@ -3935,23 +3960,23 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>375</v>
+      </c>
+      <c r="B13" t="s">
         <v>376</v>
-      </c>
-      <c r="B13" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -3959,39 +3984,39 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>383</v>
+      </c>
+      <c r="B18" t="s">
         <v>384</v>
-      </c>
-      <c r="B18" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
@@ -3999,7 +4024,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
@@ -4007,23 +4032,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -4034,7 +4059,7 @@
         <v>231</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -4127,7 +4152,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B39" t="s">
         <v>130</v>
@@ -4135,7 +4160,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B40" t="s">
         <v>132</v>
@@ -4143,7 +4168,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B41">
         <v>4000</v>
@@ -4151,7 +4176,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B42" t="s">
         <v>135</v>
@@ -4159,7 +4184,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B43" t="s">
         <v>137</v>
@@ -4167,7 +4192,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -4175,7 +4200,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B45" t="s">
         <v>66</v>
@@ -4183,7 +4208,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B46" t="s">
         <v>142</v>
@@ -4191,7 +4216,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B47" t="s">
         <v>143</v>
@@ -4199,7 +4224,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>147</v>
@@ -4207,7 +4232,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B49" t="s">
         <v>145</v>
@@ -4215,7 +4240,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -4223,23 +4248,23 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>255</v>
+      </c>
+      <c r="B51" t="s">
         <v>256</v>
-      </c>
-      <c r="B51" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>257</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B53" t="s">
         <v>145</v>
@@ -4247,7 +4272,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B55" t="s">
         <v>114</v>
@@ -4255,7 +4280,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
@@ -4263,7 +4288,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B57" t="s">
         <v>116</v>
@@ -4271,7 +4296,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -4279,7 +4304,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B59" t="s">
         <v>25</v>
@@ -4287,7 +4312,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B60" t="s">
         <v>195</v>
@@ -4295,7 +4320,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>117</v>
@@ -4303,7 +4328,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B62">
         <v>1237771234</v>
@@ -4311,7 +4336,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B63" t="s">
         <v>122</v>
@@ -4319,7 +4344,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
@@ -4327,7 +4352,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B65" t="s">
         <v>124</v>
@@ -4335,7 +4360,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B66" t="s">
         <v>118</v>
@@ -4343,7 +4368,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B67" t="s">
         <v>119</v>
@@ -4351,7 +4376,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -4359,7 +4384,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B69" t="s">
         <v>162</v>
@@ -4367,7 +4392,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B70" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
centralise the error message check
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="489">
   <si>
     <t>ITB/10000002</t>
   </si>
@@ -1479,6 +1479,24 @@
   </si>
   <si>
     <t>Fnol_Step2_MainContactNewPersonRelation</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_ReportedByInsured</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_Confirm_Homephone</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_Confirm_Mobile</t>
+  </si>
+  <si>
+    <t>ivechanged@yahoo.co.uk</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_Confirm_Email</t>
+  </si>
+  <si>
+    <t>Fnol_Step2_Confirm_HasChanges</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1528,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1523,8 +1541,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1532,12 +1574,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1556,15 +1697,137 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1840,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I275"/>
+  <dimension ref="A1:I279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1929,7 +2192,7 @@
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="b">
+      <c r="B10" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1937,7 +2200,7 @@
       <c r="A11" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="12" t="b">
+      <c r="B11" s="25" t="b">
         <v>1</v>
       </c>
       <c r="C11" t="s">
@@ -1948,7 +2211,7 @@
       <c r="A12" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="B12" s="14" t="b">
+      <c r="B12" s="38" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="s">
@@ -1959,7 +2222,7 @@
       <c r="A13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="12" t="b">
+      <c r="B13" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1967,7 +2230,7 @@
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="12" t="b">
+      <c r="B14" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1975,7 +2238,7 @@
       <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="12" t="b">
+      <c r="B15" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1983,7 +2246,7 @@
       <c r="A16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="12" t="b">
+      <c r="B16" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1991,7 +2254,7 @@
       <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="12" t="b">
+      <c r="B17" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1999,7 +2262,7 @@
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="12" t="b">
+      <c r="B18" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2007,7 +2270,7 @@
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="12" t="b">
+      <c r="B19" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2015,7 +2278,7 @@
       <c r="A20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="b">
+      <c r="B20" s="25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2023,7 +2286,7 @@
       <c r="A21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="b">
+      <c r="B21" s="25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2031,7 +2294,7 @@
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B22" t="b">
+      <c r="B22" s="25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2085,543 +2348,543 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="B32" t="b">
-        <v>1</v>
+      <c r="B32" s="17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="17" t="s">
         <v>448</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="17" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="17" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="17" t="s">
         <v>453</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="18" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="17" t="s">
         <v>455</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="17" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="A38" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="17" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="15" t="s">
         <v>458</v>
       </c>
-      <c r="B39" t="b">
+      <c r="B39" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="15" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="15" t="s">
         <v>460</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="15">
         <v>1912450444</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="16" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="A43" s="15" t="s">
         <v>464</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="15" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="15" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="A45" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="15" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="B46" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="B46" s="2" t="str">
+      <c r="B47" s="20" t="str">
         <f>B4</f>
         <v>Test Sprint5</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="8" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="22" t="s">
+        <v>488</v>
+      </c>
+      <c r="B48" s="42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="22" t="s">
         <v>467</v>
       </c>
-      <c r="B47">
+      <c r="B49" s="15">
         <v>1912859999</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="8" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="B50" s="15">
+        <v>1912840399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="22" t="s">
+        <v>485</v>
+      </c>
+      <c r="B51" s="16">
+        <v>7771234567</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="22" t="s">
         <v>468</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" s="15" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="B49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="B54" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="17" t="s">
         <v>409</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B55" s="17" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="15" t="s">
         <v>471</v>
       </c>
-      <c r="B51" t="b">
+      <c r="B56" s="15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B57" s="15" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B58" s="15" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="15" t="s">
         <v>474</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B59" s="15" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B60" s="16" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B61" s="15" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="15" t="s">
         <v>482</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B62" s="15" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="6" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>23</v>
-      </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="D64" t="s">
-        <v>264</v>
-      </c>
-      <c r="E64" t="s">
-        <v>9</v>
-      </c>
-      <c r="I64" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="D65" t="s">
-        <v>266</v>
-      </c>
-      <c r="E65" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="D66" t="s">
-        <v>267</v>
-      </c>
-      <c r="E66" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>27</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="D68" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>27</v>
-      </c>
-      <c r="B69" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="B69" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="D69" t="s">
+        <v>264</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="I69" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>31</v>
-      </c>
-      <c r="B70" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="B70" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="D70" t="s">
+        <v>266</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="I70" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>32</v>
-      </c>
-      <c r="B71" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="B71" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="D71" t="s">
+        <v>267</v>
+      </c>
+      <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>36</v>
-      </c>
-      <c r="B74" t="s">
-        <v>40</v>
+      <c r="A74" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>37</v>
-      </c>
-      <c r="B75" t="s">
-        <v>41</v>
+      <c r="A75" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B81" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79" s="6" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="6" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A80" s="8" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="B80" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="8" t="s">
+      <c r="B84" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B85" s="15" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="8" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B86" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="8" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B87" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="8" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="B84">
+      <c r="B88">
         <v>17000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>106</v>
-      </c>
-      <c r="B85" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>91</v>
-      </c>
-      <c r="B86" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>317</v>
-      </c>
-      <c r="B87" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>313</v>
-      </c>
-      <c r="B89" t="b">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="B89" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>314</v>
-      </c>
-      <c r="B90">
-        <v>125.66</v>
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>315</v>
-      </c>
-      <c r="B91">
-        <v>13</v>
+        <v>317</v>
+      </c>
+      <c r="B91" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B93" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B94" s="15">
+        <v>125.66</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B95" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="B92">
+      <c r="B96" s="15">
         <v>2476.44</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="6" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" s="6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="8" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B94" s="1" t="str">
+      <c r="B98" s="1" t="str">
         <f>B7</f>
         <v>23/01/2019</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>269</v>
-      </c>
-      <c r="B95" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>270</v>
-      </c>
-      <c r="B96" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>271</v>
-      </c>
-      <c r="B97" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B98" t="b">
-        <v>1</v>
-      </c>
-    </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>274</v>
-      </c>
-      <c r="B99" t="s">
-        <v>275</v>
+        <v>269</v>
+      </c>
+      <c r="B99" s="9">
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B100" t="b">
         <v>1</v>
@@ -2629,153 +2892,153 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>277</v>
-      </c>
-      <c r="B101" t="b">
-        <v>0</v>
-      </c>
-      <c r="D101" t="s">
-        <v>278</v>
+        <v>271</v>
+      </c>
+      <c r="B101" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>279</v>
-      </c>
-      <c r="B102" t="s">
-        <v>280</v>
+        <v>273</v>
+      </c>
+      <c r="B102" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>274</v>
+      </c>
+      <c r="B103" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="B104" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D105" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B107" s="15" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" s="6" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" s="6" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" s="8" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="B105" s="1" t="str">
+      <c r="B109" s="1" t="str">
         <f>B7</f>
         <v>23/01/2019</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>287</v>
       </c>
-      <c r="B106" s="9">
+      <c r="B110" s="9">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>288</v>
       </c>
-      <c r="B107" s="1" t="str">
+      <c r="B111" s="1" t="str">
         <f>B7</f>
         <v>23/01/2019</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
-        <v>289</v>
-      </c>
-      <c r="B108" s="9">
-        <v>0.33680555555555558</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>290</v>
-      </c>
-      <c r="B109" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
-        <v>291</v>
-      </c>
-      <c r="B110" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>292</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>294</v>
-      </c>
-      <c r="B112" s="9" t="b">
-        <v>1</v>
+        <v>289</v>
+      </c>
+      <c r="B112" s="9">
+        <v>0.33680555555555558</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>295</v>
-      </c>
-      <c r="B113" s="10">
-        <v>3</v>
+        <v>290</v>
+      </c>
+      <c r="B113" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>296</v>
-      </c>
-      <c r="B114" s="10">
-        <v>2</v>
+      <c r="A114" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B114" s="23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>297</v>
-      </c>
-      <c r="B115" s="10" t="b">
-        <v>1</v>
+      <c r="A115" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B115" s="23" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
-        <v>298</v>
-      </c>
-      <c r="B116" s="10" t="b">
-        <v>0</v>
+      <c r="A116" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B116" s="23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>299</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
+        <v>295</v>
+      </c>
+      <c r="B117" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>300</v>
-      </c>
-      <c r="B118" t="s">
-        <v>301</v>
+        <v>296</v>
+      </c>
+      <c r="B118" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B119" s="10" t="b">
         <v>1</v>
@@ -2783,133 +3046,109 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>298</v>
+      </c>
+      <c r="B120" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B121" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B123" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B124" s="14" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="B121" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+      <c r="B125" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="B122" t="b">
+      <c r="B126" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D126" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B127" s="15" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B128" s="15" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="B125" t="b">
+      <c r="B129" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B130" s="14" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127" s="6" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A131" s="6" t="s">
         <v>333</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>326</v>
-      </c>
-      <c r="B128" t="s">
-        <v>327</v>
-      </c>
-      <c r="C128">
-        <v>5</v>
-      </c>
-      <c r="D128" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
-        <v>349</v>
-      </c>
-      <c r="B129" t="b">
-        <v>1</v>
-      </c>
-      <c r="C129">
-        <v>15</v>
-      </c>
-      <c r="D129" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>346</v>
-      </c>
-      <c r="B130" t="s">
-        <v>93</v>
-      </c>
-      <c r="C130">
-        <v>15</v>
-      </c>
-      <c r="D130" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
-        <v>347</v>
-      </c>
-      <c r="B131" t="b">
-        <v>1</v>
-      </c>
-      <c r="C131">
-        <v>25</v>
-      </c>
-      <c r="D131" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>348</v>
-      </c>
-      <c r="B132" t="b">
-        <v>0</v>
+        <v>326</v>
+      </c>
+      <c r="B132" t="s">
+        <v>327</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D132" t="s">
         <v>361</v>
@@ -2917,13 +3156,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B133" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D133" t="s">
         <v>361</v>
@@ -2931,13 +3170,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>351</v>
-      </c>
-      <c r="B134" t="b">
-        <v>0</v>
+        <v>346</v>
+      </c>
+      <c r="B134" t="s">
+        <v>93</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D134" t="s">
         <v>361</v>
@@ -2945,13 +3184,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D135" t="s">
         <v>361</v>
@@ -2959,13 +3198,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D136" t="s">
         <v>361</v>
@@ -2973,13 +3212,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D137" t="s">
         <v>361</v>
@@ -2987,13 +3226,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>361</v>
@@ -3001,13 +3240,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C139">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>361</v>
@@ -3015,13 +3254,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B140" t="b">
         <v>1</v>
       </c>
       <c r="C140">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D140" t="s">
         <v>361</v>
@@ -3029,13 +3268,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B141" t="b">
         <v>1</v>
       </c>
       <c r="C141">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D141" t="s">
         <v>361</v>
@@ -3043,7 +3282,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B142" t="b">
         <v>1</v>
@@ -3057,980 +3296,1049 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
+        <v>356</v>
+      </c>
+      <c r="B143" t="b">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>20</v>
+      </c>
+      <c r="D143" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>357</v>
+      </c>
+      <c r="B144" t="b">
+        <v>1</v>
+      </c>
+      <c r="C144">
+        <v>25</v>
+      </c>
+      <c r="D144" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>358</v>
+      </c>
+      <c r="B145" t="b">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>15</v>
+      </c>
+      <c r="D145" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>359</v>
+      </c>
+      <c r="B146" t="b">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>25</v>
+      </c>
+      <c r="D146" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>360</v>
       </c>
-      <c r="B143">
+      <c r="B147">
         <v>210</v>
       </c>
-      <c r="C143">
-        <f>SUM(C128:C142)</f>
+      <c r="C147">
+        <f>SUM(C132:C146)</f>
         <v>210</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="6" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A149" s="6" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A150" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B146" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+      <c r="B150" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A151" s="15" t="s">
         <v>433</v>
       </c>
-      <c r="B147" t="str">
+      <c r="B151" s="15" t="str">
         <f>B4</f>
         <v>Test Sprint5</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>55</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B152" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>57</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B153" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+    <row r="154" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
         <v>60</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B154" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B151" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+      <c r="B155" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B156" s="29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B157" s="29" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B158" s="29" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B155" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+      <c r="B159" s="31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A160" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B160" s="31" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+    <row r="161" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A161" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B157" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="6" t="s">
+      <c r="B161" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="6" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
-        <v>178</v>
-      </c>
-      <c r="B160" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
-        <v>179</v>
-      </c>
-      <c r="B161" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
-        <v>180</v>
-      </c>
-      <c r="B162" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
-        <v>438</v>
-      </c>
-      <c r="B163" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>203</v>
-      </c>
-      <c r="B164" t="b">
-        <v>1</v>
+        <v>178</v>
+      </c>
+      <c r="B164" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="B165" t="s">
-        <v>25</v>
+        <v>189</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>438</v>
+      </c>
+      <c r="B167" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B168" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B169" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B170" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
         <v>181</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B171" s="5" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="B168" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+      <c r="B172" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B173" s="29" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B174" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B175" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B172" t="b">
+      <c r="B176" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B177" s="34" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
+    <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A178" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="B174" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="6"/>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" s="6" t="s">
+      <c r="B178" s="33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" s="6"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" s="6" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
-        <v>69</v>
-      </c>
-      <c r="B177" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
-        <v>71</v>
-      </c>
-      <c r="B178" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>72</v>
-      </c>
-      <c r="B179">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>73</v>
-      </c>
-      <c r="B180" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B181" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B182" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>80</v>
-      </c>
-      <c r="B183" t="s">
-        <v>82</v>
+        <v>72</v>
+      </c>
+      <c r="B183">
+        <v>2017</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B184" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="B185" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B186" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B187" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>444</v>
-      </c>
-      <c r="B188" t="b">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="B188" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>105</v>
+      </c>
+      <c r="B189" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="6" t="s">
-        <v>339</v>
+      <c r="A190" t="s">
+        <v>88</v>
+      </c>
+      <c r="B190" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B191" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>61</v>
-      </c>
-      <c r="B192" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
-        <v>64</v>
-      </c>
-      <c r="B193" t="s">
-        <v>63</v>
+        <v>444</v>
+      </c>
+      <c r="B192" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
-        <v>431</v>
-      </c>
-      <c r="B194" t="s">
-        <v>432</v>
+      <c r="A194" s="6" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>207</v>
-      </c>
-      <c r="B195" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B195" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>208</v>
+        <v>61</v>
       </c>
       <c r="B196" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="B197" t="s">
-        <v>206</v>
+        <v>63</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
+        <v>431</v>
+      </c>
+      <c r="B198" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B199" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B201" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
         <v>68</v>
       </c>
-      <c r="B198" s="5" t="s">
+      <c r="B202" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B199" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
+      <c r="B203" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B204" s="29" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B205" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B206" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="B203" t="b">
+      <c r="B207" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B208" s="31" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" t="s">
+    <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A209" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="B205" t="b">
+      <c r="B209" s="33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" s="6" t="s">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" s="6" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" t="s">
-        <v>148</v>
-      </c>
-      <c r="B208" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" t="s">
-        <v>149</v>
-      </c>
-      <c r="B209" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" t="s">
-        <v>150</v>
-      </c>
-      <c r="B210" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
-        <v>437</v>
-      </c>
-      <c r="B211" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>199</v>
-      </c>
-      <c r="B212" t="b">
-        <v>1</v>
+        <v>148</v>
+      </c>
+      <c r="B212" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
       <c r="B213" t="s">
-        <v>25</v>
+        <v>156</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="B214" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
+        <v>437</v>
+      </c>
+      <c r="B215" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B216" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B217" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B218" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
         <v>151</v>
       </c>
-      <c r="B215" s="5" t="s">
+      <c r="B219" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="B216" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" t="s">
+      <c r="B220" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B221" s="29" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B222" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B223" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="B220" t="b">
+      <c r="B224" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B225" s="31" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" t="s">
+    <row r="226" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A226" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B222" t="b">
+      <c r="B226" s="33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A224" s="6" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="6" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A225" t="s">
-        <v>107</v>
-      </c>
-      <c r="B225" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A226" t="s">
-        <v>109</v>
-      </c>
-      <c r="B226" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A227" t="s">
-        <v>108</v>
-      </c>
-      <c r="B227" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A228" t="s">
-        <v>434</v>
-      </c>
-      <c r="B228" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>196</v>
-      </c>
-      <c r="B229" t="b">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B229" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>197</v>
+        <v>109</v>
       </c>
       <c r="B230" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>198</v>
+        <v>108</v>
       </c>
       <c r="B231" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>110</v>
-      </c>
-      <c r="B232" s="5" t="s">
-        <v>117</v>
+        <v>434</v>
+      </c>
+      <c r="B232" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
-        <v>120</v>
-      </c>
-      <c r="B233">
-        <v>1237771234</v>
+      <c r="A233" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B233" s="14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A234" t="s">
-        <v>121</v>
-      </c>
-      <c r="B234" t="s">
-        <v>122</v>
+      <c r="A234" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B234" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A235" t="s">
-        <v>111</v>
-      </c>
-      <c r="B235" t="b">
-        <v>1</v>
+      <c r="A235" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B235" s="14" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>123</v>
-      </c>
-      <c r="B236" t="s">
-        <v>124</v>
+        <v>110</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
+        <v>120</v>
+      </c>
+      <c r="B237">
+        <v>1237771234</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A238" t="s">
+        <v>121</v>
+      </c>
+      <c r="B238" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B239" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B240" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B241" s="29" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A238" t="s">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B242" s="29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B239" t="b">
+      <c r="B243" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A240" t="s">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B244" s="31" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
+    <row r="245" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A245" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="B241" t="b">
+      <c r="B245" s="33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243" s="6" t="s">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" s="6" t="s">
         <v>342</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244" t="s">
-        <v>129</v>
-      </c>
-      <c r="B244" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245" t="s">
-        <v>131</v>
-      </c>
-      <c r="B245" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246" t="s">
-        <v>133</v>
-      </c>
-      <c r="B246">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
-        <v>134</v>
-      </c>
-      <c r="B247" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B248" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>138</v>
-      </c>
-      <c r="B249" t="b">
-        <v>1</v>
+        <v>131</v>
+      </c>
+      <c r="B249" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>139</v>
-      </c>
-      <c r="B250" t="s">
-        <v>66</v>
+        <v>133</v>
+      </c>
+      <c r="B250">
+        <v>4000</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B251" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
+        <v>136</v>
+      </c>
+      <c r="B252" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B253" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B254" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B255" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B256" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B257" s="15" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B254" s="5" t="s">
+      <c r="B258" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B259" s="15" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A257" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A258" s="6"/>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A259" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A260" s="6"/>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" s="6"/>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" s="6"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" s="6" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A262" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A263" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B263" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A264" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A265" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" s="8" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>222</v>
+        <v>213</v>
+      </c>
+      <c r="B267" s="2">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B268" s="3" t="b">
-        <v>1</v>
+        <v>214</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B269" s="3" t="b">
-        <v>1</v>
+        <v>215</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B270" s="3" t="b">
-        <v>1</v>
+        <v>216</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" s="8" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B272" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B273" s="35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B274" s="35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="B275" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B276" s="14" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A273" s="8" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B277" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A274" s="8"/>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A275" t="s">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" s="8"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
         <v>6</v>
       </c>
-      <c r="B275" s="3" t="s">
+      <c r="B279" s="3" t="s">
         <v>407</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B198" r:id="rId1"/>
-    <hyperlink ref="B232" r:id="rId2"/>
-    <hyperlink ref="B254" r:id="rId3"/>
-    <hyperlink ref="B215" r:id="rId4"/>
-    <hyperlink ref="B167" r:id="rId5"/>
+    <hyperlink ref="B202" r:id="rId1"/>
+    <hyperlink ref="B236" r:id="rId2"/>
+    <hyperlink ref="B258" r:id="rId3"/>
+    <hyperlink ref="B219" r:id="rId4"/>
+    <hyperlink ref="B171" r:id="rId5"/>
     <hyperlink ref="B36" r:id="rId6"/>
     <hyperlink ref="B42" r:id="rId7"/>
-    <hyperlink ref="B55" r:id="rId8"/>
+    <hyperlink ref="B60" r:id="rId8"/>
+    <hyperlink ref="B51" r:id="rId9" display="ivechanged@yahoo.co.uk"/>
+    <hyperlink ref="B53" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
regression tests for error messages
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -2105,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
tryiong to fix moj problems
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="648">
   <si>
     <t>ITB/10000002</t>
   </si>
@@ -1688,15 +1688,6 @@
     <t>EditPostFnol_PedestrianInjHospOvernight</t>
   </si>
   <si>
-    <t>28/01/2019</t>
-  </si>
-  <si>
-    <t>carl robertson</t>
-  </si>
-  <si>
-    <t>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</t>
-  </si>
-  <si>
     <t>000-00-000005</t>
   </si>
   <si>
@@ -1941,6 +1932,48 @@
   </si>
   <si>
     <t>EditPostFnol_TPDriverInjHospOvernight</t>
+  </si>
+  <si>
+    <t>ITB/11000002</t>
+  </si>
+  <si>
+    <t>steve anderson</t>
+  </si>
+  <si>
+    <t>7 Fieldside, Sunderland, SR6 7LA</t>
+  </si>
+  <si>
+    <t>30/01/2019</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerAddMoj</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojType</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojCreateDate</t>
+  </si>
+  <si>
+    <t>MOJ Stage 3 Settled Infant Approval</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojInsuredLiabilityPerc</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojClaimantLiabilityPerc</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojOtherLiabilityPerc</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojLowDamages</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojHighDamages</t>
+  </si>
+  <si>
+    <t>EditPostFnol_PHPassengerMojOfferDamages</t>
   </si>
 </sst>
 </file>
@@ -1972,7 +2005,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2012,6 +2045,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2128,7 +2167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2184,11 +2223,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2606,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I280"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153:XFD153"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2632,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>260</v>
+        <v>634</v>
       </c>
       <c r="D3" t="s">
         <v>260</v>
@@ -2643,7 +2684,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>553</v>
+        <v>635</v>
       </c>
       <c r="D4" t="s">
         <v>261</v>
@@ -2665,7 +2706,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>554</v>
+        <v>636</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>263</v>
@@ -2676,7 +2717,7 @@
         <v>417</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>552</v>
+        <v>637</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -2820,7 +2861,7 @@
       </c>
       <c r="B27" s="11" t="str">
         <f>B7</f>
-        <v>28/01/2019</v>
+        <v>30/01/2019</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -2974,7 +3015,7 @@
       </c>
       <c r="B47" s="20" t="str">
         <f>B4</f>
-        <v>carl robertson</v>
+        <v>steve anderson</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -3380,7 +3421,7 @@
       </c>
       <c r="B99" s="1" t="str">
         <f>B7</f>
-        <v>28/01/2019</v>
+        <v>30/01/2019</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
@@ -3469,7 +3510,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B7</f>
-        <v>28/01/2019</v>
+        <v>30/01/2019</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
@@ -3486,7 +3527,7 @@
       </c>
       <c r="B112" s="1" t="str">
         <f>B7</f>
-        <v>28/01/2019</v>
+        <v>30/01/2019</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
@@ -3890,7 +3931,7 @@
       </c>
       <c r="B152" s="15" t="str">
         <f>B4</f>
-        <v>carl robertson</v>
+        <v>steve anderson</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
@@ -5181,15 +5222,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I188"/>
+  <dimension ref="A1:I197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
@@ -5210,7 +5251,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -5218,7 +5259,7 @@
         <v>513</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>554</v>
+        <v>636</v>
       </c>
       <c r="C4" t="s">
         <v>488</v>
@@ -5227,10 +5268,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>553</v>
+        <v>635</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -5759,12 +5800,12 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="49" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B57" s="15" t="b">
         <v>1</v>
@@ -5775,11 +5816,11 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B58" s="15" t="str">
         <f>B5</f>
-        <v>carl robertson</v>
+        <v>steve anderson</v>
       </c>
       <c r="C58" t="s">
         <v>488</v>
@@ -5787,10 +5828,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>488</v>
@@ -5798,10 +5839,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>488</v>
@@ -5809,10 +5850,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>488</v>
@@ -5820,10 +5861,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>488</v>
@@ -5831,10 +5872,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>488</v>
@@ -5842,10 +5883,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B64" s="48" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>488</v>
@@ -5853,7 +5894,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B65" s="48">
         <v>1919996666</v>
@@ -5864,7 +5905,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B66" s="25">
         <v>7771438976</v>
@@ -5875,10 +5916,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C67" t="s">
         <v>488</v>
@@ -5886,7 +5927,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B68">
         <v>1237771299</v>
@@ -5897,7 +5938,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B69" t="s">
         <v>465</v>
@@ -5908,10 +5949,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C70" t="s">
         <v>488</v>
@@ -5919,10 +5960,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B71" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C71" t="s">
         <v>488</v>
@@ -5930,10 +5971,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B72" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C72" t="s">
         <v>488</v>
@@ -5941,10 +5982,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B73" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C73" t="s">
         <v>488</v>
@@ -5952,7 +5993,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B74" t="s">
         <v>58</v>
@@ -5963,7 +6004,7 @@
     </row>
     <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B75" t="s">
         <v>59</v>
@@ -5974,7 +6015,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="26" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B76" s="27" t="b">
         <v>1</v>
@@ -5985,7 +6026,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="28" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B77" s="29" t="s">
         <v>102</v>
@@ -5996,7 +6037,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B78" s="29" t="s">
         <v>128</v>
@@ -6007,7 +6048,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="28" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>103</v>
@@ -6018,7 +6059,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="30" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B80" s="31" t="b">
         <v>1</v>
@@ -6029,7 +6070,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="30" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>162</v>
@@ -6040,7 +6081,7 @@
     </row>
     <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="32" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B82" s="33" t="b">
         <v>1</v>
@@ -6055,15 +6096,15 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="51" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C85" s="25" t="s">
         <v>488</v>
@@ -6071,10 +6112,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C86" s="25" t="s">
         <v>488</v>
@@ -6082,10 +6123,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C87" s="25" t="s">
         <v>488</v>
@@ -6093,10 +6134,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C88" s="25" t="s">
         <v>488</v>
@@ -6104,10 +6145,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C89" s="25" t="s">
         <v>488</v>
@@ -6115,10 +6156,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B90" s="48" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C90" s="25" t="s">
         <v>488</v>
@@ -6126,7 +6167,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B91" s="48">
         <v>1919996666</v>
@@ -6137,7 +6178,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B92" s="25">
         <v>7771438976</v>
@@ -6148,10 +6189,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C93" t="s">
         <v>488</v>
@@ -6159,7 +6200,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B94">
         <v>1237771299</v>
@@ -6170,7 +6211,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B95" t="s">
         <v>465</v>
@@ -6181,10 +6222,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C96" t="s">
         <v>488</v>
@@ -6192,10 +6233,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B97" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C97" t="s">
         <v>488</v>
@@ -6203,10 +6244,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B98" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C98" t="s">
         <v>488</v>
@@ -6214,10 +6255,10 @@
     </row>
     <row r="99" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B99" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C99" t="s">
         <v>488</v>
@@ -6225,7 +6266,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="26" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B100" s="27" t="b">
         <v>1</v>
@@ -6236,7 +6277,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="28" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B101" s="29" t="s">
         <v>102</v>
@@ -6247,7 +6288,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="28" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B102" s="29" t="s">
         <v>128</v>
@@ -6258,7 +6299,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="28" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B103" s="29" t="s">
         <v>103</v>
@@ -6269,7 +6310,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="30" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B104" s="31" t="b">
         <v>1</v>
@@ -6280,7 +6321,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="30" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B105" s="31" t="s">
         <v>162</v>
@@ -6291,7 +6332,7 @@
     </row>
     <row r="106" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="32" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B106" s="33" t="b">
         <v>1</v>
@@ -6306,7 +6347,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B108" t="s">
         <v>66</v>
@@ -6317,7 +6358,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B109" t="s">
         <v>189</v>
@@ -6328,7 +6369,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B110" t="s">
         <v>190</v>
@@ -6339,7 +6380,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B111" t="s">
         <v>435</v>
@@ -6350,7 +6391,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="14" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B112" s="14" t="b">
         <v>1</v>
@@ -6361,7 +6402,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="14" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B113" s="14" t="s">
         <v>25</v>
@@ -6372,7 +6413,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="14" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B114" s="14" t="s">
         <v>202</v>
@@ -6383,7 +6424,7 @@
     </row>
     <row r="115" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>191</v>
@@ -6394,7 +6435,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="26" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B116" s="27" t="b">
         <v>1</v>
@@ -6405,7 +6446,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="28" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B117" s="29" t="s">
         <v>192</v>
@@ -6416,7 +6457,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="28" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B118" s="29" t="s">
         <v>96</v>
@@ -6427,7 +6468,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="28" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B119" s="29" t="s">
         <v>97</v>
@@ -6438,7 +6479,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="30" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B120" s="31" t="b">
         <v>0</v>
@@ -6449,7 +6490,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="30" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B121" s="34" t="s">
         <v>193</v>
@@ -6460,7 +6501,7 @@
     </row>
     <row r="122" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="32" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B122" s="33" t="b">
         <v>1</v>
@@ -6469,120 +6510,120 @@
         <v>488</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="47"/>
-      <c r="B123" s="47"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="6" t="s">
+    <row r="123" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="47" t="s">
+        <v>638</v>
+      </c>
+      <c r="B123" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="C123" s="25" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="47" t="s">
+        <v>639</v>
+      </c>
+      <c r="B124" s="52" t="s">
+        <v>641</v>
+      </c>
+      <c r="C124" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="47" t="s">
+        <v>640</v>
+      </c>
+      <c r="B125" s="53" t="s">
+        <v>637</v>
+      </c>
+      <c r="C125" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>642</v>
+      </c>
+      <c r="B126" s="50">
+        <v>50</v>
+      </c>
+      <c r="C126" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>643</v>
+      </c>
+      <c r="B127" s="50">
+        <v>25</v>
+      </c>
+      <c r="C127" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>644</v>
+      </c>
+      <c r="B128" s="50">
+        <v>25</v>
+      </c>
+      <c r="C128" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>645</v>
+      </c>
+      <c r="B129" s="50">
+        <v>1000</v>
+      </c>
+      <c r="C129" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>646</v>
+      </c>
+      <c r="B130" s="50">
+        <v>2000</v>
+      </c>
+      <c r="C130" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>647</v>
+      </c>
+      <c r="B131" s="50">
+        <v>1500</v>
+      </c>
+      <c r="C131" s="50" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="50"/>
+      <c r="B132" s="50"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="6" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
-        <v>243</v>
-      </c>
-      <c r="B125" t="s">
-        <v>130</v>
-      </c>
-      <c r="C125" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
-        <v>244</v>
-      </c>
-      <c r="B126" t="s">
-        <v>132</v>
-      </c>
-      <c r="C126" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
-        <v>245</v>
-      </c>
-      <c r="B127">
-        <v>4000</v>
-      </c>
-      <c r="C127" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>246</v>
-      </c>
-      <c r="B128" t="s">
-        <v>135</v>
-      </c>
-      <c r="C128" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
-        <v>247</v>
-      </c>
-      <c r="B129" t="s">
-        <v>137</v>
-      </c>
-      <c r="C129" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>248</v>
-      </c>
-      <c r="B130" t="b">
-        <v>1</v>
-      </c>
-      <c r="C130" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
-        <v>249</v>
-      </c>
-      <c r="B131" t="s">
-        <v>66</v>
-      </c>
-      <c r="C131" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
-        <v>250</v>
-      </c>
-      <c r="B132" t="s">
-        <v>142</v>
-      </c>
-      <c r="C132" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
-        <v>251</v>
-      </c>
-      <c r="B133" t="s">
-        <v>143</v>
-      </c>
-      <c r="C133" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>252</v>
-      </c>
-      <c r="B134" s="5" t="s">
-        <v>147</v>
+        <v>243</v>
+      </c>
+      <c r="B134" t="s">
+        <v>130</v>
       </c>
       <c r="C134" t="s">
         <v>488</v>
@@ -6590,10 +6631,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B135" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C135" t="s">
         <v>488</v>
@@ -6601,10 +6642,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>254</v>
-      </c>
-      <c r="B136" t="b">
-        <v>1</v>
+        <v>245</v>
+      </c>
+      <c r="B136">
+        <v>4000</v>
       </c>
       <c r="C136" t="s">
         <v>488</v>
@@ -6612,10 +6653,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B137" t="s">
-        <v>256</v>
+        <v>135</v>
       </c>
       <c r="C137" t="s">
         <v>488</v>
@@ -6623,10 +6664,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>257</v>
-      </c>
-      <c r="B138" s="5" t="s">
-        <v>258</v>
+        <v>247</v>
+      </c>
+      <c r="B138" t="s">
+        <v>137</v>
       </c>
       <c r="C138" t="s">
         <v>488</v>
@@ -6634,26 +6675,43 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>259</v>
-      </c>
-      <c r="B139" t="s">
-        <v>145</v>
+        <v>248</v>
+      </c>
+      <c r="B139" t="b">
+        <v>1</v>
       </c>
       <c r="C139" t="s">
         <v>488</v>
       </c>
     </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>249</v>
+      </c>
+      <c r="B140" t="s">
+        <v>66</v>
+      </c>
+      <c r="C140" t="s">
+        <v>488</v>
+      </c>
+    </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="6" t="s">
-        <v>530</v>
+      <c r="A141" t="s">
+        <v>250</v>
+      </c>
+      <c r="B141" t="s">
+        <v>142</v>
+      </c>
+      <c r="C141" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>387</v>
+        <v>251</v>
       </c>
       <c r="B142" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="C142" t="s">
         <v>488</v>
@@ -6661,10 +6719,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>388</v>
-      </c>
-      <c r="B143" t="s">
-        <v>115</v>
+        <v>252</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="C143" t="s">
         <v>488</v>
@@ -6672,10 +6730,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>389</v>
+        <v>253</v>
       </c>
       <c r="B144" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="C144" t="s">
         <v>488</v>
@@ -6683,7 +6741,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>390</v>
+        <v>254</v>
       </c>
       <c r="B145" t="b">
         <v>1</v>
@@ -6694,10 +6752,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>391</v>
+        <v>255</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>256</v>
       </c>
       <c r="C146" t="s">
         <v>488</v>
@@ -6705,10 +6763,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>392</v>
-      </c>
-      <c r="B147" t="s">
-        <v>195</v>
+        <v>257</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="C147" t="s">
         <v>488</v>
@@ -6716,43 +6774,26 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>393</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>117</v>
+        <v>259</v>
+      </c>
+      <c r="B148" t="s">
+        <v>145</v>
       </c>
       <c r="C148" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
-        <v>394</v>
-      </c>
-      <c r="B149">
-        <v>1237771234</v>
-      </c>
-      <c r="C149" t="s">
-        <v>488</v>
-      </c>
-    </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
-        <v>395</v>
-      </c>
-      <c r="B150" t="s">
-        <v>122</v>
-      </c>
-      <c r="C150" t="s">
-        <v>488</v>
+      <c r="A150" s="6" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>396</v>
-      </c>
-      <c r="B151" t="b">
-        <v>1</v>
+        <v>387</v>
+      </c>
+      <c r="B151" t="s">
+        <v>114</v>
       </c>
       <c r="C151" t="s">
         <v>488</v>
@@ -6760,10 +6801,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B152" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C152" t="s">
         <v>488</v>
@@ -6771,10 +6812,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B153" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C153" t="s">
         <v>488</v>
@@ -6782,10 +6823,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>399</v>
-      </c>
-      <c r="B154" t="s">
-        <v>119</v>
+        <v>390</v>
+      </c>
+      <c r="B154" t="b">
+        <v>1</v>
       </c>
       <c r="C154" t="s">
         <v>488</v>
@@ -6793,10 +6834,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>400</v>
-      </c>
-      <c r="B155" t="b">
-        <v>1</v>
+        <v>391</v>
+      </c>
+      <c r="B155" t="s">
+        <v>25</v>
       </c>
       <c r="C155" t="s">
         <v>488</v>
@@ -6804,10 +6845,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B156" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="C156" t="s">
         <v>488</v>
@@ -6815,29 +6856,32 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>402</v>
-      </c>
-      <c r="B157" t="b">
-        <v>0</v>
+        <v>393</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="C157" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" s="6" t="s">
-        <v>532</v>
+      <c r="A158" t="s">
+        <v>394</v>
+      </c>
+      <c r="B158">
+        <v>1237771234</v>
       </c>
       <c r="C158" t="s">
-        <v>559</v>
+        <v>488</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>536</v>
+        <v>395</v>
       </c>
       <c r="B159" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C159" t="s">
         <v>488</v>
@@ -6845,10 +6889,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>537</v>
-      </c>
-      <c r="B160" t="s">
-        <v>533</v>
+        <v>396</v>
+      </c>
+      <c r="B160" t="b">
+        <v>1</v>
       </c>
       <c r="C160" t="s">
         <v>488</v>
@@ -6856,54 +6900,54 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>538</v>
+        <v>397</v>
       </c>
       <c r="B161" t="s">
-        <v>534</v>
+        <v>124</v>
       </c>
       <c r="C161" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="15" t="s">
-        <v>539</v>
-      </c>
-      <c r="B162" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="C162" s="15" t="s">
-        <v>487</v>
+      <c r="A162" t="s">
+        <v>398</v>
+      </c>
+      <c r="B162" t="s">
+        <v>118</v>
+      </c>
+      <c r="C162" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="B163" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C163" s="15" t="s">
-        <v>487</v>
+      <c r="A163" t="s">
+        <v>399</v>
+      </c>
+      <c r="B163" t="s">
+        <v>119</v>
+      </c>
+      <c r="C163" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="15" t="s">
-        <v>541</v>
-      </c>
-      <c r="B164" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="C164" s="15" t="s">
-        <v>487</v>
+      <c r="A164" t="s">
+        <v>400</v>
+      </c>
+      <c r="B164" t="b">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>542</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>117</v>
+        <v>401</v>
+      </c>
+      <c r="B165" t="s">
+        <v>162</v>
       </c>
       <c r="C165" t="s">
         <v>488</v>
@@ -6911,32 +6955,29 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>543</v>
-      </c>
-      <c r="B166">
-        <v>1237771234</v>
+        <v>402</v>
+      </c>
+      <c r="B166" t="b">
+        <v>0</v>
       </c>
       <c r="C166" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
-        <v>544</v>
-      </c>
-      <c r="B167" t="s">
-        <v>535</v>
+      <c r="A167" s="6" t="s">
+        <v>532</v>
       </c>
       <c r="C167" t="s">
-        <v>488</v>
+        <v>556</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>545</v>
-      </c>
-      <c r="B168" t="b">
-        <v>1</v>
+        <v>536</v>
+      </c>
+      <c r="B168" t="s">
+        <v>114</v>
       </c>
       <c r="C168" t="s">
         <v>488</v>
@@ -6944,10 +6985,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="B169" t="s">
-        <v>558</v>
+        <v>533</v>
       </c>
       <c r="C169" t="s">
         <v>488</v>
@@ -6955,161 +6996,161 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="B170" t="s">
-        <v>556</v>
+        <v>534</v>
       </c>
       <c r="C170" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>548</v>
-      </c>
-      <c r="B171" t="s">
-        <v>557</v>
-      </c>
-      <c r="C171" t="s">
-        <v>488</v>
+      <c r="A171" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="B171" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C171" s="15" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
-        <v>549</v>
-      </c>
-      <c r="B172" t="b">
-        <v>0</v>
-      </c>
-      <c r="C172" t="s">
-        <v>488</v>
+      <c r="A172" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="B172" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C172" s="15" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
-        <v>550</v>
-      </c>
-      <c r="B173" t="s">
-        <v>162</v>
-      </c>
-      <c r="C173" t="s">
-        <v>488</v>
+      <c r="A173" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="B173" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C173" s="15" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>542</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C174" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>543</v>
+      </c>
+      <c r="B175">
+        <v>1237771234</v>
+      </c>
+      <c r="C175" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>544</v>
+      </c>
+      <c r="B176" t="s">
+        <v>535</v>
+      </c>
+      <c r="C176" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>545</v>
+      </c>
+      <c r="B177" t="b">
+        <v>1</v>
+      </c>
+      <c r="C177" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>546</v>
+      </c>
+      <c r="B178" t="s">
+        <v>555</v>
+      </c>
+      <c r="C178" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>547</v>
+      </c>
+      <c r="B179" t="s">
+        <v>553</v>
+      </c>
+      <c r="C179" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>548</v>
+      </c>
+      <c r="B180" t="s">
+        <v>554</v>
+      </c>
+      <c r="C180" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>549</v>
+      </c>
+      <c r="B181" t="b">
+        <v>0</v>
+      </c>
+      <c r="C181" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>550</v>
+      </c>
+      <c r="B182" t="s">
+        <v>162</v>
+      </c>
+      <c r="C182" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
         <v>551</v>
       </c>
-      <c r="B174" t="b">
+      <c r="B183" t="b">
         <v>0</v>
       </c>
-      <c r="C174" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176" s="6" t="s">
+      <c r="C183" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" s="6" t="s">
         <v>528</v>
-      </c>
-      <c r="C176" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="C177" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A178" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B178" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C178" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C179" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C180" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C181" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C182" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="B183" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C183" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="B184" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C184" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="B185" s="3" t="b">
-        <v>1</v>
       </c>
       <c r="C185" t="s">
         <v>488</v>
@@ -7117,10 +7158,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="8" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>225</v>
+        <v>362</v>
       </c>
       <c r="C186" t="s">
         <v>488</v>
@@ -7128,10 +7169,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="B187" t="s">
-        <v>228</v>
+        <v>232</v>
+      </c>
+      <c r="B187" s="2">
+        <v>0.41666666666666669</v>
       </c>
       <c r="C187" t="s">
         <v>488</v>
@@ -7139,12 +7180,111 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C188" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C189" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A190" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C190" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C191" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B192" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C192" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B193" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C193" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B194" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C194" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C195" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B196" t="s">
+        <v>228</v>
+      </c>
+      <c r="C196" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B197" t="s">
         <v>230</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C197" t="s">
         <v>488</v>
       </c>
     </row>
@@ -7193,7 +7333,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B108:B123">
+  <conditionalFormatting sqref="B108:B132">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -7216,12 +7356,12 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B134" r:id="rId1"/>
-    <hyperlink ref="B138" r:id="rId2"/>
-    <hyperlink ref="B148" r:id="rId3"/>
+    <hyperlink ref="B143" r:id="rId1"/>
+    <hyperlink ref="B147" r:id="rId2"/>
+    <hyperlink ref="B157" r:id="rId3"/>
     <hyperlink ref="B50" r:id="rId4"/>
     <hyperlink ref="B42" r:id="rId5"/>
-    <hyperlink ref="B165" r:id="rId6"/>
+    <hyperlink ref="B174" r:id="rId6"/>
     <hyperlink ref="B67" r:id="rId7"/>
     <hyperlink ref="B115" r:id="rId8"/>
     <hyperlink ref="B70" r:id="rId9"/>

</xml_diff>

<commit_message>
story50 new services tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="policydata" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2579" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="698">
   <si>
     <t>Fnol_PolicyNumber</t>
   </si>
@@ -2039,13 +2039,6 @@
     <t>This is where the policy data info is picked up from by the rest of the sheets</t>
   </si>
   <si>
-    <t>ITB/12000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
-carl robertson</t>
-  </si>
-  <si>
     <t>000-00-000007</t>
   </si>
   <si>
@@ -2077,6 +2070,63 @@
   </si>
   <si>
     <t>Hit in rear by third party vehicle whilst waiting to enter roundabout</t>
+  </si>
+  <si>
+    <t>ITB/12000006</t>
+  </si>
+  <si>
+    <t>simon fells</t>
+  </si>
+  <si>
+    <t>30 Baden Powell Street, Gateshead, NE9 5LD</t>
+  </si>
+  <si>
+    <t>10/02/2019</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceRequired</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceRelatedTo</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceRequestType</t>
+  </si>
+  <si>
+    <t>Perform Service</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceToPerformFilter</t>
+  </si>
+  <si>
+    <t>Car Rental</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceAddInstructions</t>
+  </si>
+  <si>
+    <t>Can you rent a car to this person</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceRequestedCompletionDate</t>
+  </si>
+  <si>
+    <t>11/03/2019</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceCustomerContact</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceAddress</t>
+  </si>
+  <si>
+    <t>enterprise rent-a-car</t>
+  </si>
+  <si>
+    <t>Fnol_Step4_OtherServiceVendorSearch</t>
   </si>
 </sst>
 </file>
@@ -6420,7 +6470,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6456,18 +6506,18 @@
         <v>660</v>
       </c>
       <c r="B5" s="98" t="s">
-        <v>668</v>
+        <v>679</v>
       </c>
       <c r="C5" s="98" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>661</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>669</v>
+        <v>680</v>
       </c>
       <c r="C6" s="98" t="s">
         <v>634</v>
@@ -6489,7 +6539,7 @@
         <v>663</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>536</v>
+        <v>681</v>
       </c>
       <c r="C8" s="98" t="s">
         <v>635</v>
@@ -6500,7 +6550,7 @@
         <v>664</v>
       </c>
       <c r="B9" s="101" t="s">
-        <v>666</v>
+        <v>682</v>
       </c>
       <c r="C9" s="101" t="s">
         <v>666</v>
@@ -6550,7 +6600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A163" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -6564,7 +6614,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -6572,7 +6622,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -6612,14 +6662,14 @@
       </c>
       <c r="B8" s="56" t="str">
         <f>IF(B4="DEV",D8,E8)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="C8" t="s">
         <v>644</v>
       </c>
       <c r="D8" s="85" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E8" s="82" t="str">
         <f>policydata!C5</f>
@@ -6632,16 +6682,14 @@
       </c>
       <c r="B9" s="82" t="str">
         <f>IF(B4="DEV",D9,E9)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="C9" t="s">
         <v>643</v>
       </c>
       <c r="D9" s="85" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E9" s="82" t="str">
         <f>policydata!C6</f>
@@ -6674,14 +6722,14 @@
       </c>
       <c r="B11" s="82" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="C11" t="s">
         <v>644</v>
       </c>
       <c r="D11" s="85" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E11" s="82" t="str">
         <f>policydata!C8</f>
@@ -6694,14 +6742,14 @@
       </c>
       <c r="B12" s="83" t="str">
         <f>IF(B4="DEV",D12,E12)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="C12" t="s">
         <v>644</v>
       </c>
       <c r="D12" s="85" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E12" s="82" t="str">
         <f>policydata!C9</f>
@@ -6852,7 +6900,7 @@
       </c>
       <c r="B32" s="80" t="str">
         <f>B12</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6878,8 +6926,7 @@
       </c>
       <c r="B36" s="81" t="str">
         <f>B9</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -6982,7 +7029,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D48" t="s">
         <v>258</v>
@@ -7037,7 +7084,7 @@
       </c>
       <c r="B55" s="80" t="str">
         <f>B12</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -7060,7 +7107,7 @@
       </c>
       <c r="B58" s="80" t="str">
         <f>B12</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -7108,8 +7155,7 @@
       </c>
       <c r="B65" s="84" t="str">
         <f>B9</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -7813,13 +7859,13 @@
     <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B160" s="60"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>1</v>
@@ -7827,7 +7873,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>0</v>
@@ -7835,7 +7881,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>0</v>
@@ -7843,7 +7889,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>0</v>
@@ -7851,7 +7897,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B165" s="30" t="b">
         <v>0</v>
@@ -7859,7 +7905,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B166" s="30" t="b">
         <v>0</v>
@@ -7867,7 +7913,7 @@
     </row>
     <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A167" s="31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B167" s="32" t="b">
         <v>0</v>
@@ -8196,10 +8242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I292"/>
+  <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285:XFD292"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="A301" sqref="A301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8221,7 +8267,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -8256,11 +8302,11 @@
       </c>
       <c r="B7" s="98" t="str">
         <f>IF(B4="DEV",D7,E7)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="D7" s="100" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E7" s="98" t="str">
         <f>policydata!C5</f>
@@ -8273,13 +8319,11 @@
       </c>
       <c r="B8" s="98" t="str">
         <f>IF(B4="DEV",D8,E8)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="D8" s="98" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E8" s="98" t="str">
         <f>policydata!C6</f>
@@ -8309,11 +8353,11 @@
       </c>
       <c r="B10" s="98" t="str">
         <f>IF(B4="DEV",D10,E10)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="D10" s="98" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E10" s="98" t="str">
         <f>policydata!C8</f>
@@ -8326,11 +8370,11 @@
       </c>
       <c r="B11" s="99" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="D11" s="98" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E11" s="98" t="str">
         <f>policydata!C9</f>
@@ -8454,7 +8498,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -8478,7 +8522,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -8632,8 +8676,7 @@
       </c>
       <c r="B51" s="19" t="str">
         <f>B8</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -9039,7 +9082,7 @@
       </c>
       <c r="B103" s="1" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -9128,7 +9171,7 @@
       </c>
       <c r="B114" s="1" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -9145,7 +9188,7 @@
       </c>
       <c r="B116" s="1" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -9549,8 +9592,7 @@
       </c>
       <c r="B156" s="14" t="str">
         <f>B8</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
@@ -10484,12 +10526,12 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" s="6" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" s="14" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B286" s="14" t="b">
         <v>1</v>
@@ -10497,7 +10539,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" s="14" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B287" s="14" t="b">
         <v>1</v>
@@ -10505,7 +10547,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" s="14" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B288" s="14" t="b">
         <v>1</v>
@@ -10513,7 +10555,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" s="14" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B289" s="14" t="b">
         <v>1</v>
@@ -10521,7 +10563,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" s="14" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B290" s="14" t="b">
         <v>1</v>
@@ -10529,7 +10571,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" s="14" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B291" s="14" t="b">
         <v>1</v>
@@ -10537,10 +10579,84 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" s="14" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B292" s="14" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="B293" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" s="13" t="s">
+        <v>684</v>
+      </c>
+      <c r="B294" s="13" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" s="13" t="s">
+        <v>688</v>
+      </c>
+      <c r="B295" s="13" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" s="13" t="s">
+        <v>686</v>
+      </c>
+      <c r="B296" s="13" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" s="13" t="s">
+        <v>690</v>
+      </c>
+      <c r="B297" s="13" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" s="13" t="s">
+        <v>692</v>
+      </c>
+      <c r="B298" s="36" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" s="13" t="s">
+        <v>694</v>
+      </c>
+      <c r="B299" s="13" t="str">
+        <f>B8</f>
+        <v>simon fells</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" s="13" t="s">
+        <v>695</v>
+      </c>
+      <c r="B300" s="13" t="str">
+        <f>B10</f>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301" s="13" t="s">
+        <v>697</v>
+      </c>
+      <c r="B301" s="13" t="s">
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -10658,7 +10774,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -12806,7 +12922,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -12846,14 +12962,14 @@
       </c>
       <c r="B8" s="56" t="str">
         <f>IF(B4="DEV",D8,E8)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="C8" t="s">
         <v>644</v>
       </c>
       <c r="D8" s="85" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E8" s="82" t="str">
         <f>policydata!C5</f>
@@ -12866,16 +12982,14 @@
       </c>
       <c r="B9" s="82" t="str">
         <f>IF(B4="DEV",D9,E9)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="C9" t="s">
         <v>643</v>
       </c>
       <c r="D9" s="85" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E9" s="82" t="str">
         <f>policydata!C6</f>
@@ -12908,14 +13022,14 @@
       </c>
       <c r="B11" s="82" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="C11" t="s">
         <v>644</v>
       </c>
       <c r="D11" s="85" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E11" s="82" t="str">
         <f>policydata!C8</f>
@@ -12928,14 +13042,14 @@
       </c>
       <c r="B12" s="83" t="str">
         <f>IF(B4="DEV",D12,E12)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="C12" t="s">
         <v>644</v>
       </c>
       <c r="D12" s="85" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E12" s="82" t="str">
         <f>policydata!C9</f>
@@ -13086,7 +13200,7 @@
       </c>
       <c r="B32" s="80" t="str">
         <f>B12</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13112,8 +13226,7 @@
       </c>
       <c r="B36" s="81" t="str">
         <f>B9</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -13271,7 +13384,7 @@
       </c>
       <c r="B55" s="80" t="str">
         <f>B12</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -13294,7 +13407,7 @@
       </c>
       <c r="B58" s="80" t="str">
         <f>B12</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -13342,8 +13455,7 @@
       </c>
       <c r="B65" s="84" t="str">
         <f>B9</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -14047,13 +14159,13 @@
     <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B160" s="60"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>1</v>
@@ -14061,7 +14173,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>0</v>
@@ -14069,7 +14181,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>0</v>
@@ -14077,7 +14189,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>0</v>
@@ -14085,7 +14197,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B165" s="30" t="b">
         <v>0</v>
@@ -14093,7 +14205,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B166" s="30" t="b">
         <v>0</v>
@@ -14101,7 +14213,7 @@
     </row>
     <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A167" s="31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B167" s="32" t="b">
         <v>0</v>
@@ -14483,11 +14595,11 @@
       </c>
       <c r="B6" s="82" t="str">
         <f>IF(B2="DEV",D6,E6)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="D6" s="85" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E6" s="82" t="str">
         <f>policydata!C5</f>
@@ -14500,13 +14612,11 @@
       </c>
       <c r="B7" s="82" t="str">
         <f>IF(B2="DEV",D7,E7)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="D7" s="85" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E7" s="82" t="str">
         <f>policydata!C6</f>
@@ -14536,11 +14646,11 @@
       </c>
       <c r="B9" s="82" t="str">
         <f>IF(B2="DEV",D9,E9)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="D9" s="85" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E9" s="82" t="str">
         <f>policydata!C8</f>
@@ -14553,11 +14663,11 @@
       </c>
       <c r="B10" s="83" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="D10" s="85" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E10" s="82" t="str">
         <f>policydata!C9</f>
@@ -14698,7 +14808,7 @@
       </c>
       <c r="B28" s="80" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -14724,8 +14834,7 @@
       </c>
       <c r="B32" s="81" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -14856,7 +14965,7 @@
       </c>
       <c r="B51" s="90" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -14879,7 +14988,7 @@
       </c>
       <c r="B54" s="90" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -14930,8 +15039,7 @@
       </c>
       <c r="B62" s="62" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -15582,8 +15690,7 @@
       </c>
       <c r="B149" s="91" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="C149" t="s">
         <v>653</v>
@@ -15651,13 +15758,13 @@
     <row r="157" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B158" s="60"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B159" s="30" t="b">
         <v>1</v>
@@ -15665,7 +15772,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B160" s="30" t="b">
         <v>0</v>
@@ -15673,7 +15780,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>0</v>
@@ -15681,7 +15788,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>0</v>
@@ -15689,7 +15796,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>0</v>
@@ -15697,7 +15804,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>0</v>
@@ -15705,7 +15812,7 @@
     </row>
     <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A165" s="31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B165" s="32" t="b">
         <v>0</v>
@@ -16057,11 +16164,11 @@
       </c>
       <c r="B7" s="93" t="str">
         <f>IF(B3="DEV",D7,E7)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="D7" s="95" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E7" s="93" t="str">
         <f>policydata!C5</f>
@@ -16074,13 +16181,11 @@
       </c>
       <c r="B8" s="93" t="str">
         <f>IF(B3="DEV",D8,E8)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="D8" s="95" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E8" s="93" t="str">
         <f>policydata!C6</f>
@@ -16110,11 +16215,11 @@
       </c>
       <c r="B10" s="93" t="str">
         <f>IF(B3="DEV",D10,E10)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="D10" s="95" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E10" s="93" t="str">
         <f>policydata!C8</f>
@@ -16127,11 +16232,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B3="DEV",D11,E11)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="D11" s="95" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>policydata!C9</f>
@@ -16279,7 +16384,7 @@
       </c>
       <c r="B31" s="96" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -16305,8 +16410,7 @@
       </c>
       <c r="B35" s="97" t="str">
         <f>B8</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -16437,7 +16541,7 @@
       </c>
       <c r="B54" s="96" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -16460,7 +16564,7 @@
       </c>
       <c r="B57" s="96" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -16508,8 +16612,7 @@
       </c>
       <c r="B64" s="28" t="str">
         <f>B8</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -17207,13 +17310,13 @@
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B159" s="60"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B160" s="30" t="b">
         <v>1</v>
@@ -17221,7 +17324,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>0</v>
@@ -17229,7 +17332,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>0</v>
@@ -17237,7 +17340,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>0</v>
@@ -17245,7 +17348,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>0</v>
@@ -17253,7 +17356,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B165" s="30" t="b">
         <v>0</v>
@@ -17261,7 +17364,7 @@
     </row>
     <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" s="31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B166" s="32" t="b">
         <v>0</v>
@@ -17591,11 +17694,11 @@
       </c>
       <c r="B7" s="98" t="str">
         <f>IF(B3="DEV",D7,E7)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="D7" s="100" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E7" s="98" t="str">
         <f>policydata!C5</f>
@@ -17608,13 +17711,11 @@
       </c>
       <c r="B8" s="98" t="str">
         <f>IF(B3="DEV",D8,E8)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="D8" s="100" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E8" s="98" t="str">
         <f>policydata!C6</f>
@@ -17644,11 +17745,11 @@
       </c>
       <c r="B10" s="98" t="str">
         <f>IF(B3="DEV",D10,E10)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="D10" s="100" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E10" s="98" t="str">
         <f>policydata!C8</f>
@@ -17661,11 +17762,11 @@
       </c>
       <c r="B11" s="99" t="str">
         <f>IF(B3="DEV",D11,E11)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="D11" s="100" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E11" s="98" t="str">
         <f>policydata!C9</f>
@@ -17813,7 +17914,7 @@
       </c>
       <c r="B31" s="96" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -17839,8 +17940,7 @@
       </c>
       <c r="B35" s="97" t="str">
         <f>B8</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -17971,7 +18071,7 @@
       </c>
       <c r="B54" s="96" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -17994,7 +18094,7 @@
       </c>
       <c r="B57" s="96" t="str">
         <f>B11</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -18042,8 +18142,7 @@
       </c>
       <c r="B64" s="28" t="str">
         <f>B8</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -18741,13 +18840,13 @@
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B159" s="60"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B160" s="30" t="b">
         <v>1</v>
@@ -18755,7 +18854,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>0</v>
@@ -18763,7 +18862,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>0</v>
@@ -18771,7 +18870,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>0</v>
@@ -18779,7 +18878,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>0</v>
@@ -18787,7 +18886,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B165" s="30" t="b">
         <v>0</v>
@@ -18795,7 +18894,7 @@
     </row>
     <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" s="31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B166" s="32" t="b">
         <v>0</v>
@@ -19133,11 +19232,11 @@
       </c>
       <c r="B6" s="98" t="str">
         <f>IF(B2="DEV",D6,E6)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="D6" s="100" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E6" s="98" t="str">
         <f>policydata!C5</f>
@@ -19150,13 +19249,11 @@
       </c>
       <c r="B7" s="98" t="str">
         <f>IF(B2="DEV",D7,E7)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="D7" s="100" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E7" s="98" t="str">
         <f>policydata!C6</f>
@@ -19186,11 +19283,11 @@
       </c>
       <c r="B9" s="98" t="str">
         <f>IF(B2="DEV",D9,E9)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="D9" s="100" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E9" s="98" t="str">
         <f>policydata!C8</f>
@@ -19203,11 +19300,11 @@
       </c>
       <c r="B10" s="99" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="D10" s="100" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E10" s="98" t="str">
         <f>policydata!C9</f>
@@ -19345,7 +19442,7 @@
       </c>
       <c r="B28" s="96" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -19371,8 +19468,7 @@
       </c>
       <c r="B32" s="97" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -19503,7 +19599,7 @@
       </c>
       <c r="B51" s="96" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -19526,7 +19622,7 @@
       </c>
       <c r="B54" s="96" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -19577,8 +19673,7 @@
       </c>
       <c r="B62" s="28" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -20284,13 +20379,13 @@
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B158" s="60"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B159" s="30" t="b">
         <v>1</v>
@@ -20298,7 +20393,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B160" s="30" t="b">
         <v>0</v>
@@ -20306,7 +20401,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>0</v>
@@ -20314,7 +20409,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>0</v>
@@ -20322,7 +20417,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>0</v>
@@ -20330,7 +20425,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>0</v>
@@ -20338,7 +20433,7 @@
     </row>
     <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A165" s="31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B165" s="32" t="b">
         <v>0</v>
@@ -20709,11 +20804,11 @@
       </c>
       <c r="B6" s="98" t="str">
         <f>IF(B2="DEV",D6,E6)</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="D6" s="100" t="str">
         <f>policydata!B5</f>
-        <v>ITB/12000000</v>
+        <v>ITB/12000006</v>
       </c>
       <c r="E6" s="98" t="str">
         <f>policydata!C5</f>
@@ -20726,13 +20821,11 @@
       </c>
       <c r="B7" s="98" t="str">
         <f>IF(B2="DEV",D7,E7)</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="D7" s="100" t="str">
         <f>policydata!B6</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
       <c r="E7" s="98" t="str">
         <f>policydata!C6</f>
@@ -20762,11 +20855,11 @@
       </c>
       <c r="B9" s="98" t="str">
         <f>IF(B2="DEV",D9,E9)</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="D9" s="100" t="str">
         <f>policydata!B8</f>
-        <v>1 Bowes Gardens, Springwell, Gateshead, NE9 7NZ</v>
+        <v>30 Baden Powell Street, Gateshead, NE9 5LD</v>
       </c>
       <c r="E9" s="98" t="str">
         <f>policydata!C8</f>
@@ -20779,11 +20872,11 @@
       </c>
       <c r="B10" s="99" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="D10" s="100" t="str">
         <f>policydata!B9</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
       <c r="E10" s="98" t="str">
         <f>policydata!C9</f>
@@ -20921,7 +21014,7 @@
       </c>
       <c r="B28" s="96" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -20947,8 +21040,7 @@
       </c>
       <c r="B32" s="97" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -21079,7 +21171,7 @@
       </c>
       <c r="B51" s="96" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -21102,7 +21194,7 @@
       </c>
       <c r="B54" s="96" t="str">
         <f>B10</f>
-        <v>07/02/2019</v>
+        <v>10/02/2019</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -21153,8 +21245,7 @@
       </c>
       <c r="B62" s="28" t="str">
         <f>B7</f>
-        <v xml:space="preserve"> 
-carl robertson</v>
+        <v>simon fells</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -21860,13 +21951,13 @@
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="59" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B158" s="60"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B159" s="30" t="b">
         <v>1</v>
@@ -21874,7 +21965,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B160" s="30" t="b">
         <v>1</v>
@@ -21882,7 +21973,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B161" s="30" t="b">
         <v>1</v>
@@ -21890,7 +21981,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B162" s="30" t="b">
         <v>1</v>
@@ -21898,7 +21989,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B163" s="30" t="b">
         <v>1</v>
@@ -21906,7 +21997,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B164" s="30" t="b">
         <v>1</v>
@@ -21914,7 +22005,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B165" s="30" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
changes for story 477
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5581" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5572" uniqueCount="831">
   <si>
     <t>Fnol_PolicyNumber</t>
   </si>
@@ -2377,9 +2377,6 @@
     <t>9 Elmsford Grove, Newcastle upon Tyne, NE12 8HT</t>
   </si>
   <si>
-    <t>21/02/2019</t>
-  </si>
-  <si>
     <t>Currently Under Investigations with SIU</t>
   </si>
   <si>
@@ -2527,7 +2524,13 @@
     <t>Non fault</t>
   </si>
   <si>
-    <t>000-00-000158</t>
+    <t>vrn lookup now</t>
+  </si>
+  <si>
+    <t>25/02/2019</t>
+  </si>
+  <si>
+    <t>000-00-000226</t>
   </si>
 </sst>
 </file>
@@ -9566,7 +9569,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9646,7 +9649,7 @@
         <v>660</v>
       </c>
       <c r="B9" s="96" t="s">
-        <v>779</v>
+        <v>829</v>
       </c>
       <c r="C9" s="96" t="s">
         <v>662</v>
@@ -9815,11 +9818,11 @@
       </c>
       <c r="B10" s="78" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D10" s="80" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E10" s="77" t="str">
         <f>POLICYDATA!C9</f>
@@ -9960,7 +9963,7 @@
       </c>
       <c r="B28" s="75" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10125,7 +10128,7 @@
       </c>
       <c r="B52" s="85" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -10148,7 +10151,7 @@
       </c>
       <c r="B55" s="85" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -11606,11 +11609,11 @@
       </c>
       <c r="B11" s="89" t="str">
         <f>IF(B3="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="90" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="88" t="str">
         <f>POLICYDATA!C9</f>
@@ -11758,7 +11761,7 @@
       </c>
       <c r="B31" s="91" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11923,7 +11926,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -11946,7 +11949,7 @@
       </c>
       <c r="B58" s="91" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -13358,11 +13361,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B3="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="95" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -13510,7 +13513,7 @@
       </c>
       <c r="B31" s="91" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13675,7 +13678,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -13698,7 +13701,7 @@
       </c>
       <c r="B58" s="91" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -15118,11 +15121,11 @@
       </c>
       <c r="B10" s="94" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D10" s="95" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E10" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -15260,7 +15263,7 @@
       </c>
       <c r="B28" s="91" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -15425,7 +15428,7 @@
       </c>
       <c r="B52" s="91" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -15448,7 +15451,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -16912,11 +16915,11 @@
       </c>
       <c r="B10" s="94" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D10" s="95" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E10" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -17054,7 +17057,7 @@
       </c>
       <c r="B28" s="91" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -17219,7 +17222,7 @@
       </c>
       <c r="B52" s="91" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -17242,7 +17245,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B10</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -18733,14 +18736,14 @@
       </c>
       <c r="B12" s="78" t="str">
         <f>IF(B4="DEV",D12,E12)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="C12" t="s">
         <v>640</v>
       </c>
       <c r="D12" s="80" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E12" s="77" t="str">
         <f>POLICYDATA!C9</f>
@@ -18891,7 +18894,7 @@
       </c>
       <c r="B32" s="75" t="str">
         <f>B12</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -19083,7 +19086,7 @@
       </c>
       <c r="B56" s="75" t="str">
         <f>B12</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -19106,7 +19109,7 @@
       </c>
       <c r="B59" s="75" t="str">
         <f>B12</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -20458,7 +20461,7 @@
   <dimension ref="A1:I354"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20472,7 +20475,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -20480,7 +20483,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C2" t="s">
         <v>721</v>
@@ -20586,11 +20589,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -20738,7 +20741,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -21044,7 +21047,7 @@
         <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -21069,7 +21072,7 @@
         <v>6</v>
       </c>
       <c r="B75" s="106" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D75" t="s">
         <v>255</v>
@@ -21103,7 +21106,7 @@
         <v>714</v>
       </c>
       <c r="B77" s="104" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D77" t="s">
         <v>357</v>
@@ -21152,7 +21155,7 @@
         <v>29</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -21315,7 +21318,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -21404,7 +21407,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -21421,7 +21424,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -21969,7 +21972,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>174</v>
       </c>
@@ -21977,7 +21980,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="24" t="s">
         <v>175</v>
       </c>
@@ -21985,7 +21988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="26" t="s">
         <v>176</v>
       </c>
@@ -21993,7 +21996,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="26" t="s">
         <v>177</v>
       </c>
@@ -22001,7 +22004,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="26" t="s">
         <v>178</v>
       </c>
@@ -22009,7 +22012,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="28" t="s">
         <v>179</v>
       </c>
@@ -22017,7 +22020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="28" t="s">
         <v>180</v>
       </c>
@@ -22025,7 +22028,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="30" t="s">
         <v>181</v>
       </c>
@@ -22033,15 +22036,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="6"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>63</v>
       </c>
@@ -22049,61 +22052,46 @@
         <v>64</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>65</v>
       </c>
       <c r="B188" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C188" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>66</v>
       </c>
-      <c r="B189">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>67</v>
       </c>
-      <c r="B190" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>68</v>
       </c>
-      <c r="B191" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>72</v>
-      </c>
-      <c r="B192" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>74</v>
       </c>
-      <c r="B193" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>75</v>
       </c>
-      <c r="B194" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
@@ -23238,7 +23226,7 @@
         <v>705</v>
       </c>
       <c r="B348" s="103" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -23484,8 +23472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I354"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23499,7 +23487,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -23613,11 +23601,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -23765,7 +23753,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -24071,7 +24059,7 @@
         <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -24096,7 +24084,7 @@
         <v>6</v>
       </c>
       <c r="B75" s="106" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D75" t="s">
         <v>255</v>
@@ -24113,7 +24101,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="107" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D76" t="s">
         <v>256</v>
@@ -24130,7 +24118,7 @@
         <v>714</v>
       </c>
       <c r="B77" s="104" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D77" t="s">
         <v>357</v>
@@ -24179,7 +24167,7 @@
         <v>29</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -24342,7 +24330,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -24431,7 +24419,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -24448,7 +24436,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -25088,49 +25076,31 @@
       <c r="A189" t="s">
         <v>66</v>
       </c>
-      <c r="B189">
-        <v>2017</v>
-      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>67</v>
       </c>
-      <c r="B190" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>68</v>
       </c>
-      <c r="B191" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>72</v>
       </c>
-      <c r="B192" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>74</v>
       </c>
-      <c r="B193" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>75</v>
       </c>
-      <c r="B194" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
@@ -26265,7 +26235,7 @@
         <v>705</v>
       </c>
       <c r="B348" s="103" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -26511,7 +26481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I354"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
@@ -26526,7 +26496,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -26632,11 +26602,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -26691,7 +26661,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -26787,7 +26757,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -27082,7 +27052,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D72" t="s">
         <v>254</v>
@@ -27093,7 +27063,7 @@
         <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -27135,7 +27105,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="107" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D76" t="s">
         <v>256</v>
@@ -27177,7 +27147,7 @@
         <v>24</v>
       </c>
       <c r="B79" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -27292,7 +27262,7 @@
         <v>100</v>
       </c>
       <c r="B95" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -27300,7 +27270,7 @@
         <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -27360,7 +27330,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -27384,7 +27354,7 @@
         <v>260</v>
       </c>
       <c r="B107" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -27427,7 +27397,7 @@
         <v>268</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -27449,7 +27419,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -27466,7 +27436,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -27878,7 +27848,7 @@
         <v>49</v>
       </c>
       <c r="B158" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
@@ -27918,7 +27888,7 @@
         <v>121</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -27926,7 +27896,7 @@
         <v>98</v>
       </c>
       <c r="B164" s="102" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -29283,7 +29253,7 @@
         <v>705</v>
       </c>
       <c r="B348" s="103" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -29544,7 +29514,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -29650,11 +29620,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -29802,7 +29772,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -29851,7 +29821,7 @@
         <v>427</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -29859,7 +29829,7 @@
         <v>429</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -29867,7 +29837,7 @@
         <v>431</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -29875,7 +29845,7 @@
         <v>433</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -29883,7 +29853,7 @@
         <v>424</v>
       </c>
       <c r="B42" s="98" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -30097,7 +30067,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D72" t="s">
         <v>254</v>
@@ -30108,7 +30078,7 @@
         <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -30300,7 +30270,7 @@
         <v>100</v>
       </c>
       <c r="B95" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -30308,7 +30278,7 @@
         <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -30365,7 +30335,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -30389,7 +30359,7 @@
         <v>260</v>
       </c>
       <c r="B107" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -30432,7 +30402,7 @@
         <v>268</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -30454,7 +30424,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -30471,7 +30441,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -30503,7 +30473,7 @@
         <v>281</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -30559,7 +30529,7 @@
         <v>289</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
@@ -30883,7 +30853,7 @@
         <v>49</v>
       </c>
       <c r="B158" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
@@ -30923,7 +30893,7 @@
         <v>121</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -30931,7 +30901,7 @@
         <v>98</v>
       </c>
       <c r="B164" s="102" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -32288,7 +32258,7 @@
         <v>705</v>
       </c>
       <c r="B348" s="103" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -32547,7 +32517,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -32653,11 +32623,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -32805,7 +32775,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -33100,7 +33070,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D72" t="s">
         <v>254</v>
@@ -33111,7 +33081,7 @@
         <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -33136,7 +33106,7 @@
         <v>6</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D75" t="s">
         <v>255</v>
@@ -33153,7 +33123,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="107" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D76" t="s">
         <v>256</v>
@@ -33187,7 +33157,7 @@
         <v>22</v>
       </c>
       <c r="B78" s="101" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -33195,7 +33165,7 @@
         <v>24</v>
       </c>
       <c r="B79" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -33306,7 +33276,7 @@
         <v>100</v>
       </c>
       <c r="B95" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -33314,7 +33284,7 @@
         <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -33374,7 +33344,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -33398,7 +33368,7 @@
         <v>260</v>
       </c>
       <c r="B107" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -33441,7 +33411,7 @@
         <v>268</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -33463,7 +33433,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -33480,7 +33450,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -33892,7 +33862,7 @@
         <v>49</v>
       </c>
       <c r="B158" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
@@ -33932,7 +33902,7 @@
         <v>121</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -33940,7 +33910,7 @@
         <v>98</v>
       </c>
       <c r="B164" s="102" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -35297,7 +35267,7 @@
         <v>705</v>
       </c>
       <c r="B348" s="103" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -35558,7 +35528,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -35664,11 +35634,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -35816,7 +35786,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -36111,7 +36081,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D72" t="s">
         <v>254</v>
@@ -36122,7 +36092,7 @@
         <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -36198,7 +36168,7 @@
         <v>22</v>
       </c>
       <c r="B78" s="101" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -36206,7 +36176,7 @@
         <v>24</v>
       </c>
       <c r="B79" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -36317,7 +36287,7 @@
         <v>100</v>
       </c>
       <c r="B95" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -36325,7 +36295,7 @@
         <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -36385,7 +36355,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -36409,7 +36379,7 @@
         <v>260</v>
       </c>
       <c r="B107" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -36452,7 +36422,7 @@
         <v>268</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -36474,7 +36444,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -36491,7 +36461,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f>B11</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -36903,7 +36873,7 @@
         <v>49</v>
       </c>
       <c r="B158" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
@@ -36943,7 +36913,7 @@
         <v>121</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -36951,7 +36921,7 @@
         <v>98</v>
       </c>
       <c r="B164" s="102" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -38308,7 +38278,7 @@
         <v>705</v>
       </c>
       <c r="B348" s="103" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -40860,14 +40830,14 @@
       </c>
       <c r="B12" s="78" t="str">
         <f>IF(B4="DEV",D12,E12)</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="C12" t="s">
         <v>640</v>
       </c>
       <c r="D12" s="80" t="str">
         <f>POLICYDATA!B9</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
       <c r="E12" s="77" t="str">
         <f>POLICYDATA!C9</f>
@@ -41018,7 +40988,7 @@
       </c>
       <c r="B32" s="75" t="str">
         <f>B12</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -41210,7 +41180,7 @@
       </c>
       <c r="B56" s="75" t="str">
         <f>B12</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -41233,7 +41203,7 @@
       </c>
       <c r="B59" s="75" t="str">
         <f>B12</f>
-        <v>21/02/2019</v>
+        <v>25/02/2019</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fix for change to TP insurer locator
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="POLICYDATA" sheetId="11" r:id="rId1"/>
@@ -2584,13 +2584,13 @@
     <t>BP Garage on the A325</t>
   </si>
   <si>
-    <t>28/02/2019</t>
-  </si>
-  <si>
     <t>Fnol_Step5_Notes</t>
   </si>
   <si>
     <t>000-00-000325</t>
+  </si>
+  <si>
+    <t>04/03/2019</t>
   </si>
 </sst>
 </file>
@@ -10483,8 +10483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10564,7 +10564,7 @@
         <v>660</v>
       </c>
       <c r="B9" s="96" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="C9" s="96" t="s">
         <v>662</v>
@@ -10733,11 +10733,11 @@
       </c>
       <c r="B10" s="78" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D10" s="80" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E10" s="77" t="str">
         <f>POLICYDATA!C9</f>
@@ -10878,7 +10878,7 @@
       </c>
       <c r="B28" s="75" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11043,7 +11043,7 @@
       </c>
       <c r="B52" s="85" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -11066,7 +11066,7 @@
       </c>
       <c r="B55" s="85" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -12524,11 +12524,11 @@
       </c>
       <c r="B11" s="89" t="str">
         <f>IF(B3="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="90" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="88" t="str">
         <f>POLICYDATA!C9</f>
@@ -12676,7 +12676,7 @@
       </c>
       <c r="B31" s="91" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12841,7 +12841,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -12864,7 +12864,7 @@
       </c>
       <c r="B58" s="91" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -14276,11 +14276,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B3="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="95" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -14428,7 +14428,7 @@
       </c>
       <c r="B31" s="91" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -14593,7 +14593,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -14616,7 +14616,7 @@
       </c>
       <c r="B58" s="91" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -16036,11 +16036,11 @@
       </c>
       <c r="B10" s="94" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D10" s="95" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E10" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -16178,7 +16178,7 @@
       </c>
       <c r="B28" s="91" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -16343,7 +16343,7 @@
       </c>
       <c r="B52" s="91" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -16366,7 +16366,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -17830,11 +17830,11 @@
       </c>
       <c r="B10" s="94" t="str">
         <f>IF(B2="DEV",D10,E10)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D10" s="95" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E10" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -17972,7 +17972,7 @@
       </c>
       <c r="B28" s="91" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -18137,7 +18137,7 @@
       </c>
       <c r="B52" s="91" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -18160,7 +18160,7 @@
       </c>
       <c r="B55" s="91" t="str">
         <f>B10</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -19651,14 +19651,14 @@
       </c>
       <c r="B12" s="78" t="str">
         <f>IF(B4="DEV",D12,E12)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="C12" t="s">
         <v>640</v>
       </c>
       <c r="D12" s="80" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E12" s="77" t="str">
         <f>POLICYDATA!C9</f>
@@ -19809,7 +19809,7 @@
       </c>
       <c r="B32" s="75" t="str">
         <f>B12</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -20001,7 +20001,7 @@
       </c>
       <c r="B56" s="75" t="str">
         <f>B12</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -20024,7 +20024,7 @@
       </c>
       <c r="B59" s="75" t="str">
         <f>B12</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -21375,8 +21375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21398,7 +21398,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C2" t="s">
         <v>723</v>
@@ -21504,11 +21504,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -21656,7 +21656,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -22272,7 +22272,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -22361,7 +22361,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -22378,7 +22378,7 @@
       </c>
       <c r="B123" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -24261,7 +24261,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B366" s="103" t="str">
         <f>B79</f>
@@ -24651,11 +24651,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -24803,7 +24803,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -25423,7 +25423,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -25512,7 +25512,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -25529,7 +25529,7 @@
       </c>
       <c r="B123" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -27409,7 +27409,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B366" s="103" t="str">
         <f>B79</f>
@@ -27857,11 +27857,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -28012,7 +28012,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -28630,7 +28630,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -28719,7 +28719,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -28736,7 +28736,7 @@
       </c>
       <c r="B123" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -30602,7 +30602,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B362" s="103" t="str">
         <f>B79</f>
@@ -31017,11 +31017,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -31169,7 +31169,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -31780,7 +31780,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -31869,7 +31869,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -31886,7 +31886,7 @@
       </c>
       <c r="B123" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -33752,7 +33752,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B362" s="103" t="str">
         <f>B79</f>
@@ -34156,11 +34156,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -34308,7 +34308,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -34922,7 +34922,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -35011,7 +35011,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -35028,7 +35028,7 @@
       </c>
       <c r="B123" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -36894,7 +36894,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B362" s="103" t="str">
         <f>B79</f>
@@ -37177,7 +37177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I362"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A331" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
@@ -37298,11 +37298,11 @@
       </c>
       <c r="B11" s="94" t="str">
         <f>IF(B4="DEV",D11,E11)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="D11" s="93" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E11" s="93" t="str">
         <f>POLICYDATA!C9</f>
@@ -37450,7 +37450,7 @@
       </c>
       <c r="B31" s="11" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -38064,7 +38064,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -38153,7 +38153,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -38170,7 +38170,7 @@
       </c>
       <c r="B123" s="1" t="str">
         <f>B11</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -40036,7 +40036,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B362" s="103" t="str">
         <f>B79</f>
@@ -42625,14 +42625,14 @@
       </c>
       <c r="B12" s="78" t="str">
         <f>IF(B4="DEV",D12,E12)</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="C12" t="s">
         <v>640</v>
       </c>
       <c r="D12" s="80" t="str">
         <f>POLICYDATA!B9</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
       <c r="E12" s="77" t="str">
         <f>POLICYDATA!C9</f>
@@ -42783,7 +42783,7 @@
       </c>
       <c r="B32" s="75" t="str">
         <f>B12</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -42975,7 +42975,7 @@
       </c>
       <c r="B56" s="75" t="str">
         <f>B12</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -42998,7 +42998,7 @@
       </c>
       <c r="B59" s="75" t="str">
         <f>B12</f>
-        <v>28/02/2019</v>
+        <v>04/03/2019</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add indemnity incidents/offences setup in fnol
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="POLICYDATA" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7357" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7370" uniqueCount="936">
   <si>
     <t>Fnol_PolicyNumber</t>
   </si>
@@ -2837,6 +2837,18 @@
   </si>
   <si>
     <t>regress_fnol_inconly</t>
+  </si>
+  <si>
+    <t>Tourist Board Employee</t>
+  </si>
+  <si>
+    <t>Zoologist</t>
+  </si>
+  <si>
+    <t>01/1/2017</t>
+  </si>
+  <si>
+    <t>Coach Builder</t>
   </si>
 </sst>
 </file>
@@ -2874,7 +2886,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2938,6 +2950,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3082,7 +3100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -3223,13 +3241,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1329">
+  <dxfs count="1332">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11925,7 +11963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -12337,90 +12375,90 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="1328" priority="31" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1327" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="1331" priority="31" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1330" priority="32" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1326" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="1329" priority="33" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F21">
-    <cfRule type="cellIs" dxfId="1325" priority="16" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1324" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1328" priority="16" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1327" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1323" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="1326" priority="18" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F19">
-    <cfRule type="cellIs" dxfId="1322" priority="19" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1321" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="1325" priority="19" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1324" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1320" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="1323" priority="21" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F11">
-    <cfRule type="cellIs" dxfId="1319" priority="13" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1318" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="1322" priority="13" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1321" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1317" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="1320" priority="15" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12 F14">
-    <cfRule type="cellIs" dxfId="1316" priority="10" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1315" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1319" priority="10" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1318" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1314" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="1317" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="1313" priority="7" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1312" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1316" priority="7" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1315" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1311" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1314" priority="9" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="1310" priority="4" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1309" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1313" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1312" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1308" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1311" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1310" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1309" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1308" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12434,7 +12472,7 @@
   <dimension ref="A1:D353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14886,8 +14924,8 @@
       <c r="A318" s="12" t="s">
         <v>654</v>
       </c>
-      <c r="B318" s="12" t="b">
-        <v>1</v>
+      <c r="B318" s="119" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
@@ -15406,8 +15444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30197,8 +30235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I372"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157:XFD164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31465,7 +31503,7 @@
         <v>51</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>52</v>
+        <v>933</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
@@ -31505,7 +31543,7 @@
         <v>836</v>
       </c>
       <c r="B157" s="111" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
@@ -31529,7 +31567,7 @@
         <v>841</v>
       </c>
       <c r="B160" s="94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -31537,7 +31575,7 @@
         <v>842</v>
       </c>
       <c r="B161" s="113" t="s">
-        <v>844</v>
+        <v>934</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -33321,7 +33359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D372"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="D340" sqref="D340"/>
     </sheetView>
   </sheetViews>
@@ -39502,10 +39540,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I353"/>
+  <dimension ref="A1:I361"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E305" sqref="E305"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40766,10 +40804,10 @@
         <v>51</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>54</v>
       </c>
@@ -40778,325 +40816,325 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A153" s="21" t="s">
+      <c r="A153" s="44" t="s">
+        <v>836</v>
+      </c>
+      <c r="B153" s="111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A154" s="44" t="s">
+        <v>837</v>
+      </c>
+      <c r="B154" s="112" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155" s="44" t="s">
+        <v>838</v>
+      </c>
+      <c r="B155" s="111" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="B156" s="94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="B157" s="113" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158" s="12" t="s">
+        <v>843</v>
+      </c>
+      <c r="B158" s="94" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="B159" s="94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A160" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="B160" s="94" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B153" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A154" s="23" t="s">
+      <c r="B161" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B154" s="96" t="s">
+      <c r="B162" s="96" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A155" s="23" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="B155" s="24" t="s">
+      <c r="B163" s="24" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A156" s="23" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B156" s="96" t="s">
+      <c r="B164" s="96" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A157" s="25" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B157" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A158" s="25" t="s">
+      <c r="B165" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="B158" s="26" t="s">
+      <c r="B166" s="26" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A159" s="27" t="s">
+    <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A167" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="B159" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="5" t="s">
+      <c r="B167" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" s="5" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
         <v>171</v>
       </c>
-      <c r="B162" s="5" t="s">
+      <c r="B170" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
         <v>172</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B171" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
         <v>173</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B172" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
         <v>414</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B173" s="5" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="11" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B166" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" s="11" t="s">
+      <c r="B174" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B167" s="11" t="s">
+      <c r="B175" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" s="11" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B168" s="97" t="s">
+      <c r="B176" s="97" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A169" t="s">
+    <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
         <v>174</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" s="21" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="B170" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" s="23" t="s">
+      <c r="B178" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="B171" s="24" t="s">
+      <c r="B179" s="24" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="23" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="B172" s="96" t="s">
+      <c r="B180" s="96" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" s="23" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B173" s="96" t="s">
+      <c r="B181" s="96" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="25" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="B174" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="25" t="s">
+      <c r="B182" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="B175" s="29" t="s">
+      <c r="B183" s="29" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A176" s="27" t="s">
+    <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A184" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="B176" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="5"/>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" s="5" t="s">
+      <c r="B184" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" s="5"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" s="5" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>63</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>65</v>
-      </c>
-      <c r="B180" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
-        <v>66</v>
-      </c>
-      <c r="B181">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
-        <v>67</v>
-      </c>
-      <c r="B182" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
-        <v>68</v>
-      </c>
-      <c r="B183" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
-        <v>72</v>
-      </c>
-      <c r="B184" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
-        <v>74</v>
-      </c>
-      <c r="B185" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
-        <v>75</v>
-      </c>
-      <c r="B186" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>711</v>
-      </c>
-      <c r="B187" t="b">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>712</v>
+        <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>713</v>
+        <v>69</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>715</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>716</v>
+        <v>66</v>
+      </c>
+      <c r="B189">
+        <v>2017</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>714</v>
-      </c>
-      <c r="B190">
-        <v>27000</v>
+        <v>67</v>
+      </c>
+      <c r="B190" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B191" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B192" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>717</v>
-      </c>
-      <c r="B193" t="b">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B193" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>83</v>
-      </c>
-      <c r="B194" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="B194" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>420</v>
+        <v>711</v>
       </c>
       <c r="B195" t="b">
         <v>1</v>
@@ -41104,1426 +41142,1501 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>633</v>
-      </c>
-      <c r="B196" t="b">
-        <v>1</v>
+        <v>712</v>
+      </c>
+      <c r="B196" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>710</v>
-      </c>
-      <c r="B197" s="5" t="str">
-        <f>B203</f>
-        <v>Roy Racer</v>
+        <v>715</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>714</v>
+      </c>
+      <c r="B198">
+        <v>27000</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" s="5" t="s">
-        <v>327</v>
+      <c r="A199" t="s">
+        <v>99</v>
+      </c>
+      <c r="B199" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>59</v>
-      </c>
-      <c r="B200" s="5" t="s">
-        <v>60</v>
+        <v>82</v>
+      </c>
+      <c r="B200" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>55</v>
-      </c>
-      <c r="B201" t="s">
-        <v>56</v>
+        <v>717</v>
+      </c>
+      <c r="B201" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>58</v>
-      </c>
-      <c r="B202" t="s">
-        <v>57</v>
+        <v>83</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
+        <v>420</v>
+      </c>
+      <c r="B203" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>633</v>
+      </c>
+      <c r="B204" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>710</v>
+      </c>
+      <c r="B205" s="5" t="str">
+        <f>B211</f>
+        <v>Roy Racer</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>59</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>55</v>
+      </c>
+      <c r="B209" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>58</v>
+      </c>
+      <c r="B210" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
         <v>407</v>
       </c>
-      <c r="B203" s="5" t="s">
+      <c r="B211" s="5" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" s="11" t="s">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B204" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" s="11" t="s">
+      <c r="B212" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B205" s="11" t="s">
+      <c r="B213" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" s="11" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B206" s="97" t="s">
+      <c r="B214" s="97" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A207" t="s">
+    <row r="215" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A215" t="s">
         <v>62</v>
       </c>
-      <c r="B207" s="4" t="s">
+      <c r="B215" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" s="21" t="s">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B208" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" s="23" t="s">
+      <c r="B216" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B209" s="24" t="s">
+      <c r="B217" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" s="23" t="s">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B210" s="96" t="s">
+      <c r="B218" s="96" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" s="23" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B211" s="96" t="s">
+      <c r="B219" s="96" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A212" s="25" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="B212" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A213" s="25" t="s">
+      <c r="B220" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="B213" s="26" t="s">
+      <c r="B221" s="26" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A214" s="27" t="s">
+    <row r="222" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A222" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="B214" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" s="5" t="s">
+      <c r="B222" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="5" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
         <v>142</v>
       </c>
-      <c r="B217" s="5" t="s">
+      <c r="B225" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" t="s">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
         <v>143</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B226" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" t="s">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
         <v>144</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B227" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
         <v>413</v>
       </c>
-      <c r="B220" s="5" t="s">
+      <c r="B228" s="5" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" s="11" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B221" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" s="11" t="s">
+      <c r="B229" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B222" s="11" t="s">
+      <c r="B230" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A223" s="11" t="s">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B223" s="97" t="s">
+      <c r="B231" s="97" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A224" t="s">
+    <row r="232" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
         <v>145</v>
       </c>
-      <c r="B224" s="4" t="s">
+      <c r="B232" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A225" s="21" t="s">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B225" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A226" s="23" t="s">
+      <c r="B233" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B226" s="24" t="s">
+      <c r="B234" s="24" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A227" s="23" t="s">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="B227" s="96" t="s">
+      <c r="B235" s="96" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A228" s="23" t="s">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="B228" s="96" t="s">
+      <c r="B236" s="96" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A229" s="25" t="s">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="B229" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A230" s="25" t="s">
+      <c r="B237" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="B230" s="26" t="s">
+      <c r="B238" s="26" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A231" s="27" t="s">
+    <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A239" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="B231" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A233" s="5" t="s">
+      <c r="B239" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="5" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A234" t="s">
-        <v>101</v>
-      </c>
-      <c r="B234" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A235" t="s">
-        <v>103</v>
-      </c>
-      <c r="B235" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A236" t="s">
-        <v>102</v>
-      </c>
-      <c r="B236" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A237" t="s">
-        <v>410</v>
-      </c>
-      <c r="B237" s="5" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A238" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B238" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B239" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A240" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B240" s="97" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
-        <v>104</v>
-      </c>
-      <c r="B241" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
+        <v>101</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>103</v>
+      </c>
+      <c r="B243" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>102</v>
+      </c>
+      <c r="B244" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>410</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B246" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B247" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B248" s="97" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>104</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
         <v>114</v>
       </c>
-      <c r="B242">
+      <c r="B250">
         <v>1237771234</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A243" t="s">
+    <row r="251" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A251" t="s">
         <v>115</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B251" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244" s="21" t="s">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B244" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245" s="23" t="s">
+      <c r="B252" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B245" s="24" t="s">
+      <c r="B253" s="24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246" s="23" t="s">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B246" s="96" t="s">
+      <c r="B254" s="96" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A247" s="23" t="s">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B247" s="96" t="s">
+      <c r="B255" s="96" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A248" s="25" t="s">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="B248" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A249" s="25" t="s">
+      <c r="B256" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B249" s="26" t="s">
+      <c r="B257" s="26" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A250" s="27" t="s">
+    <row r="258" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A258" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="B250" s="28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A252" s="5" t="s">
+      <c r="B258" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" s="5" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
         <v>123</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B261" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
         <v>125</v>
       </c>
-      <c r="B254" t="s">
+      <c r="B262" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
         <v>127</v>
       </c>
-      <c r="B255">
+      <c r="B263">
         <v>4000</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
         <v>128</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B264" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
         <v>130</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B265" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
         <v>725</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B266" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
         <v>727</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B267" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A260" t="s">
+    <row r="268" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A268" t="s">
         <v>730</v>
       </c>
-      <c r="B260" t="s">
+      <c r="B268" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A261" s="102" t="s">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="B261" s="103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A262" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="B262" s="104" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A263" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="B263" s="26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A264" s="25" t="s">
-        <v>753</v>
-      </c>
-      <c r="B264" s="26"/>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A265" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B265" s="26" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A266" s="25" t="s">
-        <v>416</v>
-      </c>
-      <c r="B266" s="104" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A267" s="25" t="s">
-        <v>757</v>
-      </c>
-      <c r="B267" s="107">
-        <v>1912850388</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A268" s="25" t="s">
-        <v>758</v>
-      </c>
-      <c r="B268" s="107">
-        <v>1912840399</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A269" s="25" t="s">
-        <v>759</v>
-      </c>
-      <c r="B269" s="107">
-        <v>7791458073</v>
+      <c r="B269" s="103" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" s="25" t="s">
-        <v>760</v>
-      </c>
-      <c r="B270" s="107"/>
+        <v>133</v>
+      </c>
+      <c r="B270" s="104" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B271" s="26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" s="25" t="s">
+        <v>753</v>
+      </c>
+      <c r="B272" s="26"/>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B273" s="26" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="B274" s="104" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" s="25" t="s">
+        <v>757</v>
+      </c>
+      <c r="B275" s="107">
+        <v>1912850388</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" s="25" t="s">
+        <v>758</v>
+      </c>
+      <c r="B276" s="107">
+        <v>1912840399</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" s="25" t="s">
+        <v>759</v>
+      </c>
+      <c r="B277" s="107">
+        <v>7791458073</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" s="25" t="s">
+        <v>760</v>
+      </c>
+      <c r="B278" s="107"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" s="25" t="s">
         <v>762</v>
       </c>
-      <c r="B271" s="104" t="s">
+      <c r="B279" s="104" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A272" s="106" t="s">
+    <row r="280" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A280" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="B272" s="26" t="s">
+      <c r="B280" s="26" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A273" s="106" t="s">
+    <row r="281" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A281" s="106" t="s">
         <v>754</v>
       </c>
-      <c r="B273" s="26" t="s">
+      <c r="B281" s="26" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A274" s="23" t="s">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282" s="23" t="s">
         <v>740</v>
       </c>
-      <c r="B274" s="24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A275" s="23" t="s">
+      <c r="B282" s="24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283" s="23" t="s">
         <v>743</v>
       </c>
-      <c r="B275" s="24" t="s">
+      <c r="B283" s="24" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A276" s="23" t="s">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284" s="23" t="s">
         <v>744</v>
       </c>
-      <c r="B276" s="24" t="s">
+      <c r="B284" s="24" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A277" s="25" t="s">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285" s="25" t="s">
         <v>731</v>
       </c>
-      <c r="B277" s="26" t="s">
+      <c r="B285" s="26" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A278" s="25" t="s">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" s="25" t="s">
         <v>733</v>
       </c>
-      <c r="B278" s="26" t="s">
+      <c r="B286" s="26" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A279" s="106" t="s">
+    <row r="287" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A287" s="106" t="s">
         <v>735</v>
       </c>
-      <c r="B279" s="105" t="s">
+      <c r="B287" s="105" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A280" s="25" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288" s="25" t="s">
         <v>737</v>
       </c>
-      <c r="B280" s="104" t="s">
+      <c r="B288" s="104" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A281" s="25" t="s">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A289" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B281" s="26" t="s">
+      <c r="B289" s="26" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A282" s="25" t="s">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A290" s="25" t="s">
         <v>745</v>
       </c>
-      <c r="B282" s="104" t="b">
-        <v>0</v>
-      </c>
-      <c r="C282" t="s">
+      <c r="B290" s="104" t="b">
+        <v>0</v>
+      </c>
+      <c r="C290" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A283" s="25" t="s">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A291" s="25" t="s">
         <v>746</v>
       </c>
-      <c r="B283" s="104" t="s">
+      <c r="B291" s="104" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A284" s="25" t="s">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A292" s="25" t="s">
         <v>748</v>
       </c>
-      <c r="B284" s="104" t="s">
+      <c r="B292" s="104" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A285" s="25" t="s">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A293" s="25" t="s">
         <v>750</v>
       </c>
-      <c r="B285" s="104">
+      <c r="B293" s="104">
         <v>99990000</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A286" s="27" t="s">
+    <row r="294" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A294" s="27" t="s">
         <v>751</v>
       </c>
-      <c r="B286" s="28">
+      <c r="B294" s="28">
         <v>990099</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A287" s="11" t="s">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A295" s="11" t="s">
         <v>718</v>
       </c>
-      <c r="B287" s="97" t="s">
+      <c r="B295" s="97" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A288" s="11" t="s">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A296" s="11" t="s">
         <v>719</v>
       </c>
-      <c r="B288" s="31">
+      <c r="B296" s="31">
         <v>3500</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A289" s="11" t="s">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A297" s="11" t="s">
         <v>720</v>
       </c>
-      <c r="B289" s="31" t="s">
+      <c r="B297" s="31" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A290" s="20" t="s">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A298" s="20" t="s">
         <v>722</v>
       </c>
-      <c r="B290" s="49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A292" s="5" t="s">
+      <c r="B298" s="49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A300" s="5" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A293" s="11" t="s">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A301" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="B293" s="11" t="s">
+      <c r="B301" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A294" s="11" t="s">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A302" s="11" t="s">
         <v>900</v>
       </c>
-      <c r="B294" s="97" t="s">
+      <c r="B302" s="97" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A295" s="11" t="s">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A303" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="B295" s="97" t="s">
+      <c r="B303" s="97" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A296" s="11" t="s">
+    <row r="304" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A304" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="B296" s="31" t="s">
+      <c r="B304" s="31" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A297" s="11" t="s">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305" s="11" t="s">
         <v>905</v>
       </c>
-      <c r="B297" s="31" t="s">
+      <c r="B305" s="31" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A298" s="11" t="s">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="B298" s="117" t="s">
+      <c r="B306" s="117" t="s">
         <v>908</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A299" s="11" t="s">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="B299" s="11" t="s">
+      <c r="B307" s="11" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A300" s="5"/>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A301" s="5" t="s">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308" s="5"/>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309" s="5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A302" s="5"/>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A303" s="5" t="s">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310" s="5"/>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311" s="5" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A304" s="7" t="s">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B304" s="2" t="s">
+      <c r="B312" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A305" s="7" t="s">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B305" s="1">
+      <c r="B313" s="1">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A306" s="7" t="s">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B306" s="2" t="s">
+      <c r="B314" s="2" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A307" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B307" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A308" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B308" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A309" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B309" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A310" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="B310" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A311" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="B311" s="30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A312" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="B312" s="30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A313" s="31" t="s">
-        <v>217</v>
-      </c>
-      <c r="B313" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A314" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="B314" s="11" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B318" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B319" s="30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A320" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B320" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A321" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="B321" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A322" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="B322" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A323" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B323" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A316" s="7"/>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A317" s="5" t="s">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A324" s="7"/>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A325" s="5" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A318" s="12" t="s">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A326" s="12" t="s">
         <v>654</v>
       </c>
-      <c r="B318" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A319" s="12" t="s">
+      <c r="B326" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A327" s="12" t="s">
         <v>655</v>
       </c>
-      <c r="B319" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A320" s="12" t="s">
+      <c r="B327" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A328" s="12" t="s">
         <v>656</v>
       </c>
-      <c r="B320" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A321" s="12" t="s">
+      <c r="B328" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A329" s="12" t="s">
         <v>657</v>
       </c>
-      <c r="B321" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A322" s="12" t="s">
+      <c r="B329" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A330" s="12" t="s">
         <v>658</v>
       </c>
-      <c r="B322" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A323" s="12" t="s">
+      <c r="B330" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A331" s="12" t="s">
         <v>659</v>
       </c>
-      <c r="B323" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A324" s="12" t="s">
+      <c r="B331" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A332" s="12" t="s">
         <v>660</v>
       </c>
-      <c r="B324" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A325" s="11" t="s">
+      <c r="B332" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A333" s="11" t="s">
         <v>663</v>
       </c>
-      <c r="B325" s="11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A326" s="11" t="s">
+      <c r="B333" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A334" s="11" t="s">
         <v>664</v>
       </c>
-      <c r="B326" s="97" t="s">
+      <c r="B334" s="97" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A327" s="11" t="s">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A335" s="11" t="s">
         <v>668</v>
       </c>
-      <c r="B327" s="11" t="s">
+      <c r="B335" s="11" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A328" s="11" t="s">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A336" s="11" t="s">
         <v>666</v>
       </c>
-      <c r="B328" s="97" t="s">
+      <c r="B336" s="97" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A329" s="11" t="s">
-        <v>670</v>
-      </c>
-      <c r="B329" s="11" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A330" s="11" t="s">
-        <v>672</v>
-      </c>
-      <c r="B330" s="32" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A331" s="11" t="s">
-        <v>676</v>
-      </c>
-      <c r="B331" s="97" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A333" s="41" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A334" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="B334" s="12" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A335" s="12" t="s">
-        <v>679</v>
-      </c>
-      <c r="B335" s="94" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A336" s="12" t="s">
-        <v>681</v>
-      </c>
-      <c r="B336" s="94"/>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" s="11" t="s">
-        <v>682</v>
+        <v>670</v>
       </c>
       <c r="B337" s="11" t="s">
-        <v>467</v>
+        <v>671</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="B338" s="97"/>
+        <v>672</v>
+      </c>
+      <c r="B338" s="32" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" s="11" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="B339" s="97" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A340" s="12" t="s">
-        <v>686</v>
-      </c>
-      <c r="B340" s="12" t="s">
-        <v>468</v>
+        <v>675</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A341" s="12" t="s">
-        <v>687</v>
-      </c>
-      <c r="B341" s="94" t="s">
-        <v>689</v>
+      <c r="A341" s="41" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" s="12" t="s">
-        <v>688</v>
-      </c>
-      <c r="B342" s="94"/>
+        <v>678</v>
+      </c>
+      <c r="B342" s="12" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A343" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="B343" s="11" t="s">
-        <v>467</v>
+      <c r="A343" s="12" t="s">
+        <v>679</v>
+      </c>
+      <c r="B343" s="94" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A344" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="B344" s="97"/>
+      <c r="A344" s="12" t="s">
+        <v>681</v>
+      </c>
+      <c r="B344" s="94"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" s="11" t="s">
-        <v>692</v>
-      </c>
-      <c r="B345" s="97" t="s">
-        <v>763</v>
+        <v>682</v>
+      </c>
+      <c r="B345" s="11" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A346" s="12" t="s">
-        <v>694</v>
-      </c>
-      <c r="B346" s="12" t="s">
-        <v>468</v>
-      </c>
+      <c r="A346" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="B346" s="97"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A347" s="12" t="s">
-        <v>695</v>
-      </c>
-      <c r="B347" s="94" t="s">
-        <v>697</v>
+      <c r="A347" s="11" t="s">
+        <v>684</v>
+      </c>
+      <c r="B347" s="97" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" s="12" t="s">
-        <v>696</v>
-      </c>
-      <c r="B348" s="94"/>
+        <v>686</v>
+      </c>
+      <c r="B348" s="12" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A349" s="11" t="s">
-        <v>698</v>
-      </c>
-      <c r="B349" s="11" t="s">
-        <v>468</v>
+      <c r="A349" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="B349" s="94" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A350" s="11" t="s">
-        <v>699</v>
-      </c>
-      <c r="B350" s="97" t="s">
-        <v>707</v>
-      </c>
+      <c r="A350" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="B350" s="94"/>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="B351" s="97"/>
+        <v>690</v>
+      </c>
+      <c r="B351" s="11" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="B352" s="97"/>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="B353" s="97" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A354" s="12" t="s">
+        <v>694</v>
+      </c>
+      <c r="B354" s="12" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A355" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="B355" s="94" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A356" s="12" t="s">
+        <v>696</v>
+      </c>
+      <c r="B356" s="94"/>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="B357" s="11" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B358" s="97" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A359" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="B359" s="97"/>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="B353" s="97" t="str">
+      <c r="B361" s="97" t="str">
         <f>B68</f>
         <v>FIRE - My car burst in flames on the hard shoulder</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B198:B257 B291:B292 B282:B286 B261:B280 B68 B354:B1048576 B352 B1:B59 B71:B72 B325:B336 B74:B195 B300:B316">
-    <cfRule type="cellIs" dxfId="1112" priority="73" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1111" priority="74" operator="equal">
+  <conditionalFormatting sqref="B206:B265 B299:B300 B290:B294 B269:B288 B68 B362:B1048576 B360 B1:B59 B71:B72 B333:B344 B74:B152 B308:B324 B161:B203">
+    <cfRule type="cellIs" dxfId="1112" priority="76" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1111" priority="77" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1110" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="1110" priority="78" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B196:B197">
-    <cfRule type="cellIs" dxfId="1109" priority="64" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1108" priority="65" operator="equal">
+  <conditionalFormatting sqref="B204:B205">
+    <cfRule type="cellIs" dxfId="1109" priority="67" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1108" priority="68" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1107" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="1107" priority="69" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B317:B324">
-    <cfRule type="cellIs" dxfId="1106" priority="61" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1105" priority="62" operator="equal">
+  <conditionalFormatting sqref="B325:B332">
+    <cfRule type="cellIs" dxfId="1106" priority="64" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1105" priority="65" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1104" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="1104" priority="66" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B337:B339">
-    <cfRule type="cellIs" dxfId="1103" priority="58" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1102" priority="59" operator="equal">
+  <conditionalFormatting sqref="B345:B347">
+    <cfRule type="cellIs" dxfId="1103" priority="61" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1102" priority="62" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1101" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="1101" priority="63" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B340:B342">
-    <cfRule type="cellIs" dxfId="1100" priority="55" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1099" priority="56" operator="equal">
+  <conditionalFormatting sqref="B348:B350">
+    <cfRule type="cellIs" dxfId="1100" priority="58" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1099" priority="59" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1098" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="1098" priority="60" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B343:B345">
-    <cfRule type="cellIs" dxfId="1097" priority="52" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1096" priority="53" operator="equal">
+  <conditionalFormatting sqref="B351:B353">
+    <cfRule type="cellIs" dxfId="1097" priority="55" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1096" priority="56" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1095" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="1095" priority="57" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B346:B348">
-    <cfRule type="cellIs" dxfId="1094" priority="49" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1093" priority="50" operator="equal">
+  <conditionalFormatting sqref="B354:B356">
+    <cfRule type="cellIs" dxfId="1094" priority="52" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1093" priority="53" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1092" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="1092" priority="54" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B349:B351">
-    <cfRule type="cellIs" dxfId="1091" priority="46" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1090" priority="47" operator="equal">
+  <conditionalFormatting sqref="B357:B359">
+    <cfRule type="cellIs" dxfId="1091" priority="49" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1090" priority="50" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1089" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="1089" priority="51" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B287">
-    <cfRule type="cellIs" dxfId="1088" priority="43" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1087" priority="44" operator="equal">
+  <conditionalFormatting sqref="B295">
+    <cfRule type="cellIs" dxfId="1088" priority="46" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1087" priority="47" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1086" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="1086" priority="48" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B288">
-    <cfRule type="cellIs" dxfId="1085" priority="40" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1084" priority="41" operator="equal">
+  <conditionalFormatting sqref="B296">
+    <cfRule type="cellIs" dxfId="1085" priority="43" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1084" priority="44" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1083" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="1083" priority="45" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B297">
+    <cfRule type="cellIs" dxfId="1082" priority="40" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1081" priority="41" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1080" priority="42" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B298">
+    <cfRule type="cellIs" dxfId="1079" priority="37" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1078" priority="38" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1077" priority="39" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B266:B268">
+    <cfRule type="cellIs" dxfId="1076" priority="34" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1075" priority="35" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1074" priority="36" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B289">
-    <cfRule type="cellIs" dxfId="1082" priority="37" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1081" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="1073" priority="31" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1072" priority="32" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1080" priority="39" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B290">
-    <cfRule type="cellIs" dxfId="1079" priority="34" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1078" priority="35" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1077" priority="36" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B258:B260">
-    <cfRule type="cellIs" dxfId="1076" priority="31" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1075" priority="32" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1074" priority="33" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B281">
-    <cfRule type="cellIs" dxfId="1073" priority="28" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1072" priority="29" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1071" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="1071" priority="33" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="cellIs" dxfId="1070" priority="25" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1069" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="1070" priority="28" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1069" priority="29" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1068" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="1068" priority="30" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="cellIs" dxfId="1067" priority="22" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1066" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="1067" priority="25" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1066" priority="26" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1065" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="1065" priority="27" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="cellIs" dxfId="1064" priority="19" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1063" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="1064" priority="22" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1063" priority="23" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1062" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="1062" priority="24" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64:B65">
-    <cfRule type="cellIs" dxfId="1061" priority="16" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1060" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1061" priority="19" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1060" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1059" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="1059" priority="21" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="cellIs" dxfId="1058" priority="13" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1057" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="1058" priority="16" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1057" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1056" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="1056" priority="18" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="cellIs" dxfId="1055" priority="10" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1054" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1055" priority="13" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1054" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1053" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="1053" priority="15" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="cellIs" dxfId="1052" priority="7" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1051" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1052" priority="10" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1051" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1050" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1050" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B353">
-    <cfRule type="cellIs" dxfId="1049" priority="4" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1048" priority="5" operator="equal">
+  <conditionalFormatting sqref="B361">
+    <cfRule type="cellIs" dxfId="1049" priority="7" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1048" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1047" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1047" priority="9" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="cellIs" dxfId="1046" priority="1" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1045" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1046" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1045" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1044" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1044" priority="6" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B153:B160">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B207" r:id="rId1"/>
-    <hyperlink ref="B241" r:id="rId2"/>
-    <hyperlink ref="B272" r:id="rId3"/>
-    <hyperlink ref="B224" r:id="rId4"/>
-    <hyperlink ref="B169" r:id="rId5"/>
+    <hyperlink ref="B215" r:id="rId1"/>
+    <hyperlink ref="B249" r:id="rId2"/>
+    <hyperlink ref="B280" r:id="rId3"/>
+    <hyperlink ref="B232" r:id="rId4"/>
+    <hyperlink ref="B177" r:id="rId5"/>
     <hyperlink ref="B30" r:id="rId6"/>
     <hyperlink ref="B36" r:id="rId7"/>
     <hyperlink ref="B53" r:id="rId8"/>
     <hyperlink ref="B44" r:id="rId9" display="ivechanged@yahoo.co.uk"/>
     <hyperlink ref="B46" r:id="rId10"/>
-    <hyperlink ref="B273" r:id="rId11"/>
-    <hyperlink ref="B298" r:id="rId12"/>
+    <hyperlink ref="B281" r:id="rId11"/>
+    <hyperlink ref="B306" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
@@ -42534,8 +42647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I353"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B302" sqref="B302"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43786,7 +43899,7 @@
         <v>51</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>52</v>
+        <v>932</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -48555,7 +48668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I353"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added tests for cheque approval
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="POLICYDATA" sheetId="11" r:id="rId1"/>
@@ -2851,7 +2851,7 @@
     <t>postfnol_set1</t>
   </si>
   <si>
-    <t>000-00-000261</t>
+    <t>000-00-000149</t>
   </si>
 </sst>
 </file>
@@ -12004,8 +12004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15492,7 +15492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -39590,8 +39590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I361"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="B371" sqref="B371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>